<commit_message>
SM 2022 - v 6 juli
</commit_message>
<xml_diff>
--- a/mallar/import/Sm2022/extr3_sm2022.xlsx
+++ b/mallar/import/Sm2022/extr3_sm2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\episerver\voltige\VoltigeClosedXML\mallar\import\Sm2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD6E51E-0DC0-4068-BDFC-9702A2EC8282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C96A340D-E8B2-4636-AD2D-60706D66E433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" tabRatio="483" activeTab="1" xr2:uid="{9C6C5895-3CBC-495A-8EC3-24DF642F0EB2}"/>
+    <workbookView xWindow="-1965" yWindow="5468" windowWidth="5400" windowHeight="3172" tabRatio="483" activeTab="1" xr2:uid="{9C6C5895-3CBC-495A-8EC3-24DF642F0EB2}"/>
   </bookViews>
   <sheets>
     <sheet name="ekipage" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="213">
   <si>
     <t>Linda Jenvall</t>
   </si>
@@ -653,6 +653,30 @@
   </si>
   <si>
     <t>2 domare.</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Team Athena</t>
+  </si>
+  <si>
+    <t>Team Cassiopeia</t>
+  </si>
+  <si>
+    <t>Team Afrodite</t>
+  </si>
+  <si>
+    <t>Team Crux</t>
+  </si>
+  <si>
+    <t>Laholm Ryttarförening</t>
+  </si>
+  <si>
+    <t>Frillesås Rid och körklubb</t>
+  </si>
+  <si>
+    <t>Billdals Ridklubb Blå</t>
   </si>
 </sst>
 </file>
@@ -676,7 +700,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -684,13 +708,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1005,10 +1051,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B3B0E3-2027-4083-B582-AAB0C4C3F786}">
-  <dimension ref="A1:V59"/>
+  <dimension ref="A1:W59"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1018,17 +1064,19 @@
     <col min="6" max="6" width="12.1328125" customWidth="1"/>
     <col min="7" max="7" width="26.59765625" customWidth="1"/>
     <col min="9" max="9" width="33.86328125" customWidth="1"/>
-    <col min="10" max="10" width="78.3984375" customWidth="1"/>
-    <col min="11" max="11" width="10.3984375" customWidth="1"/>
-    <col min="12" max="12" width="22.265625" customWidth="1"/>
-    <col min="14" max="14" width="18.265625" customWidth="1"/>
-    <col min="16" max="16" width="19.265625" customWidth="1"/>
-    <col min="18" max="18" width="22.73046875" customWidth="1"/>
-    <col min="19" max="19" width="18" customWidth="1"/>
-    <col min="22" max="22" width="9.1328125" customWidth="1"/>
+    <col min="10" max="10" width="78.3984375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="22.86328125" customWidth="1"/>
+    <col min="12" max="12" width="10.3984375" customWidth="1"/>
+    <col min="13" max="13" width="22.265625" customWidth="1"/>
+    <col min="15" max="15" width="18.265625" customWidth="1"/>
+    <col min="17" max="17" width="19.265625" customWidth="1"/>
+    <col min="19" max="19" width="22.73046875" customWidth="1"/>
+    <col min="20" max="20" width="7.1328125" customWidth="1"/>
+    <col min="21" max="21" width="15.6640625" customWidth="1"/>
+    <col min="23" max="23" width="9.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:23" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1">
         <v>571814</v>
       </c>
@@ -1039,64 +1087,67 @@
         <v>78</v>
       </c>
       <c r="D1">
-        <v>53144</v>
+        <v>65038</v>
       </c>
       <c r="E1" t="s">
-        <v>73</v>
+        <v>174</v>
       </c>
       <c r="F1">
-        <v>138736</v>
+        <v>82226</v>
       </c>
       <c r="G1" t="s">
-        <v>67</v>
+        <v>161</v>
       </c>
       <c r="H1">
-        <v>609</v>
+        <v>223</v>
       </c>
       <c r="I1" t="s">
-        <v>63</v>
-      </c>
-      <c r="J1" t="s">
-        <v>85</v>
-      </c>
-      <c r="K1">
-        <v>70336</v>
-      </c>
-      <c r="L1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M1">
-        <v>87139</v>
-      </c>
-      <c r="N1" t="s">
-        <v>44</v>
-      </c>
-      <c r="O1">
-        <v>57826</v>
-      </c>
-      <c r="P1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q1">
-        <v>34693</v>
-      </c>
-      <c r="R1" t="s">
-        <v>46</v>
-      </c>
-      <c r="S1">
-        <v>134144</v>
-      </c>
-      <c r="T1" t="s">
-        <v>47</v>
-      </c>
-      <c r="U1">
-        <v>159908</v>
-      </c>
-      <c r="V1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="K1" t="s">
+        <v>207</v>
+      </c>
+      <c r="L1">
+        <v>115495</v>
+      </c>
+      <c r="M1" t="s">
+        <v>104</v>
+      </c>
+      <c r="N1">
+        <v>163943</v>
+      </c>
+      <c r="O1" t="s">
+        <v>105</v>
+      </c>
+      <c r="P1">
+        <v>119893</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1">
+        <v>124472</v>
+      </c>
+      <c r="S1" t="s">
+        <v>106</v>
+      </c>
+      <c r="T1">
+        <v>145200</v>
+      </c>
+      <c r="U1" t="s">
+        <v>107</v>
+      </c>
+      <c r="V1">
+        <v>155344</v>
+      </c>
+      <c r="W1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>571814</v>
       </c>
@@ -1107,64 +1158,67 @@
         <v>78</v>
       </c>
       <c r="D2">
-        <v>68838</v>
+        <v>53144</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="F2">
-        <v>7110</v>
+        <v>138736</v>
       </c>
       <c r="G2" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="H2">
-        <v>875</v>
+        <v>609</v>
       </c>
       <c r="I2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2" t="s">
-        <v>86</v>
-      </c>
-      <c r="K2">
-        <v>36794</v>
-      </c>
-      <c r="L2" t="s">
-        <v>33</v>
-      </c>
-      <c r="M2">
-        <v>164089</v>
-      </c>
-      <c r="N2" t="s">
-        <v>36</v>
-      </c>
-      <c r="O2">
-        <v>82678</v>
-      </c>
-      <c r="P2" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q2">
-        <v>51513</v>
-      </c>
-      <c r="R2" t="s">
-        <v>37</v>
-      </c>
-      <c r="S2">
-        <v>108189</v>
-      </c>
-      <c r="T2" t="s">
-        <v>34</v>
-      </c>
-      <c r="U2">
-        <v>105337</v>
-      </c>
-      <c r="V2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.45">
+        <v>63</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K2" t="s">
+        <v>210</v>
+      </c>
+      <c r="L2">
+        <v>70336</v>
+      </c>
+      <c r="M2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2">
+        <v>87139</v>
+      </c>
+      <c r="O2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P2">
+        <v>57826</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>45</v>
+      </c>
+      <c r="R2">
+        <v>34693</v>
+      </c>
+      <c r="S2" t="s">
+        <v>46</v>
+      </c>
+      <c r="T2">
+        <v>134144</v>
+      </c>
+      <c r="U2" t="s">
+        <v>47</v>
+      </c>
+      <c r="V2">
+        <v>159908</v>
+      </c>
+      <c r="W2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>571814</v>
       </c>
@@ -1175,64 +1229,67 @@
         <v>78</v>
       </c>
       <c r="D3">
-        <v>65038</v>
+        <v>68838</v>
       </c>
       <c r="E3" t="s">
-        <v>174</v>
+        <v>40</v>
       </c>
       <c r="F3">
-        <v>82226</v>
+        <v>7110</v>
       </c>
       <c r="G3" t="s">
-        <v>161</v>
+        <v>39</v>
       </c>
       <c r="H3">
-        <v>223</v>
+        <v>875</v>
       </c>
       <c r="I3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" t="s">
-        <v>184</v>
-      </c>
-      <c r="K3">
-        <v>115495</v>
-      </c>
-      <c r="L3" t="s">
-        <v>104</v>
-      </c>
-      <c r="M3">
-        <v>163943</v>
-      </c>
-      <c r="N3" t="s">
-        <v>105</v>
-      </c>
-      <c r="O3">
-        <v>119893</v>
-      </c>
-      <c r="P3" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q3">
-        <v>124472</v>
-      </c>
-      <c r="R3" t="s">
-        <v>106</v>
-      </c>
-      <c r="S3">
-        <v>145200</v>
-      </c>
-      <c r="T3" t="s">
-        <v>107</v>
-      </c>
-      <c r="U3">
-        <v>155344</v>
-      </c>
-      <c r="V3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="K3" t="s">
+        <v>206</v>
+      </c>
+      <c r="L3">
+        <v>51513</v>
+      </c>
+      <c r="M3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3">
+        <v>108189</v>
+      </c>
+      <c r="O3" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3">
+        <v>82678</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>35</v>
+      </c>
+      <c r="R3">
+        <v>36794</v>
+      </c>
+      <c r="S3" t="s">
+        <v>33</v>
+      </c>
+      <c r="T3">
+        <v>105337</v>
+      </c>
+      <c r="U3" t="s">
+        <v>49</v>
+      </c>
+      <c r="V3">
+        <v>164089</v>
+      </c>
+      <c r="W3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>571814</v>
       </c>
@@ -1260,44 +1317,44 @@
       <c r="I4" t="s">
         <v>157</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>22011</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>109</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>38926</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>110</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>139839</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>111</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>68718</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>112</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>128776</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>113</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>107006</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>571815</v>
       </c>
@@ -1325,47 +1382,47 @@
       <c r="I5" t="s">
         <v>158</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>129485</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>115</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>108087</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>116</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>134138</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>117</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>129079</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>118</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>107961</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>119</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <v>129688</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>571815</v>
       </c>
@@ -1376,64 +1433,67 @@
         <v>79</v>
       </c>
       <c r="D6">
-        <v>68838</v>
+        <v>18663</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>178</v>
       </c>
       <c r="F6">
-        <v>137228</v>
+        <v>120239</v>
       </c>
       <c r="G6" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="H6">
-        <v>875</v>
+        <v>594</v>
       </c>
       <c r="I6" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" t="s">
-        <v>186</v>
-      </c>
-      <c r="K6">
-        <v>120375</v>
-      </c>
-      <c r="L6" t="s">
-        <v>121</v>
-      </c>
-      <c r="M6">
-        <v>129183</v>
-      </c>
-      <c r="N6" t="s">
-        <v>122</v>
-      </c>
-      <c r="O6">
-        <v>107737</v>
-      </c>
-      <c r="P6" t="s">
-        <v>123</v>
-      </c>
-      <c r="Q6">
-        <v>140351</v>
-      </c>
-      <c r="R6" t="s">
-        <v>124</v>
-      </c>
-      <c r="S6">
-        <v>123591</v>
-      </c>
-      <c r="T6" t="s">
-        <v>125</v>
-      </c>
-      <c r="U6">
-        <v>127857</v>
-      </c>
-      <c r="V6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.45">
+        <v>159</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="L6">
+        <v>151413</v>
+      </c>
+      <c r="M6" t="s">
+        <v>128</v>
+      </c>
+      <c r="N6">
+        <v>152057</v>
+      </c>
+      <c r="O6" t="s">
+        <v>129</v>
+      </c>
+      <c r="P6">
+        <v>164002</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>130</v>
+      </c>
+      <c r="R6">
+        <v>155756</v>
+      </c>
+      <c r="S6" t="s">
+        <v>131</v>
+      </c>
+      <c r="T6">
+        <v>160046</v>
+      </c>
+      <c r="U6" t="s">
+        <v>132</v>
+      </c>
+      <c r="V6">
+        <v>140835</v>
+      </c>
+      <c r="W6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>571815</v>
       </c>
@@ -1461,47 +1521,50 @@
       <c r="I7" t="s">
         <v>2</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="K7">
+      <c r="K7" t="s">
+        <v>209</v>
+      </c>
+      <c r="L7">
         <v>74165</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>19</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>69830</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>41</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>109403</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>20</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>101580</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>127</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <v>129881</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>98</v>
       </c>
-      <c r="U7">
+      <c r="V7">
         <v>145224</v>
       </c>
-      <c r="V7" t="s">
+      <c r="W7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:23" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>571815</v>
       </c>
@@ -1512,84 +1575,87 @@
         <v>79</v>
       </c>
       <c r="D8">
-        <v>18663</v>
+        <v>68838</v>
       </c>
       <c r="E8" t="s">
-        <v>178</v>
+        <v>40</v>
       </c>
       <c r="F8">
-        <v>120239</v>
+        <v>137228</v>
       </c>
       <c r="G8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H8">
-        <v>594</v>
+        <v>875</v>
       </c>
       <c r="I8" t="s">
-        <v>159</v>
-      </c>
-      <c r="J8" t="s">
-        <v>188</v>
-      </c>
-      <c r="K8">
-        <v>151413</v>
-      </c>
-      <c r="L8" t="s">
-        <v>128</v>
-      </c>
-      <c r="M8">
-        <v>152057</v>
-      </c>
-      <c r="N8" t="s">
-        <v>129</v>
-      </c>
-      <c r="O8">
-        <v>164002</v>
-      </c>
-      <c r="P8" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q8">
-        <v>155756</v>
-      </c>
-      <c r="R8" t="s">
-        <v>131</v>
-      </c>
-      <c r="S8">
-        <v>160046</v>
-      </c>
-      <c r="T8" t="s">
-        <v>132</v>
-      </c>
-      <c r="U8">
-        <v>140835</v>
-      </c>
-      <c r="V8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="K8" t="s">
+        <v>208</v>
+      </c>
+      <c r="L8">
+        <v>107737</v>
+      </c>
+      <c r="M8" t="s">
+        <v>123</v>
+      </c>
+      <c r="N8">
+        <v>129183</v>
+      </c>
+      <c r="O8" t="s">
+        <v>122</v>
+      </c>
+      <c r="P8">
+        <v>127857</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>126</v>
+      </c>
+      <c r="R8">
+        <v>120375</v>
+      </c>
+      <c r="S8" t="s">
+        <v>121</v>
+      </c>
+      <c r="T8">
+        <v>140351</v>
+      </c>
+      <c r="U8" t="s">
+        <v>124</v>
+      </c>
+      <c r="V8">
+        <v>123591</v>
+      </c>
+      <c r="W8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A9">
-        <v>571816</v>
+        <v>571818</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D9">
-        <v>69289</v>
+        <v>59650</v>
       </c>
       <c r="E9" t="s">
-        <v>74</v>
+        <v>181</v>
       </c>
       <c r="F9">
-        <v>126785</v>
+        <v>81536</v>
       </c>
       <c r="G9" t="s">
-        <v>68</v>
+        <v>170</v>
       </c>
       <c r="H9">
         <v>609</v>
@@ -1597,236 +1663,239 @@
       <c r="I9" t="s">
         <v>63</v>
       </c>
-      <c r="J9" t="s">
-        <v>87</v>
-      </c>
-      <c r="K9">
-        <v>35251</v>
-      </c>
-      <c r="L9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="J9" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="L9">
+        <v>60750</v>
+      </c>
+      <c r="M9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A10">
-        <v>571816</v>
+        <v>571818</v>
       </c>
       <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10">
+        <v>39883</v>
+      </c>
+      <c r="E10" t="s">
+        <v>176</v>
+      </c>
+      <c r="F10">
+        <v>139483</v>
+      </c>
+      <c r="G10" t="s">
+        <v>163</v>
+      </c>
+      <c r="H10">
+        <v>1198</v>
+      </c>
+      <c r="I10" t="s">
+        <v>158</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="L10">
+        <v>108087</v>
+      </c>
+      <c r="M10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>571818</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11">
+        <v>39883</v>
+      </c>
+      <c r="E11" t="s">
+        <v>176</v>
+      </c>
+      <c r="F11">
+        <v>139483</v>
+      </c>
+      <c r="G11" t="s">
+        <v>163</v>
+      </c>
+      <c r="H11">
+        <v>1198</v>
+      </c>
+      <c r="I11" t="s">
+        <v>158</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="L11">
+        <v>134138</v>
+      </c>
+      <c r="M11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>571819</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12">
+        <v>39883</v>
+      </c>
+      <c r="E12" t="s">
+        <v>176</v>
+      </c>
+      <c r="F12">
+        <v>44643</v>
+      </c>
+      <c r="G12" t="s">
+        <v>171</v>
+      </c>
+      <c r="H12">
+        <v>1198</v>
+      </c>
+      <c r="I12" t="s">
+        <v>158</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="L12">
+        <v>129688</v>
+      </c>
+      <c r="M12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>571819</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13">
+        <v>39883</v>
+      </c>
+      <c r="E13" t="s">
+        <v>176</v>
+      </c>
+      <c r="F13">
+        <v>44643</v>
+      </c>
+      <c r="G13" t="s">
+        <v>171</v>
+      </c>
+      <c r="H13">
+        <v>1198</v>
+      </c>
+      <c r="I13" t="s">
+        <v>158</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="L13">
+        <v>129079</v>
+      </c>
+      <c r="M13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>571818</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14">
+        <v>40552</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14">
+        <v>133740</v>
+      </c>
+      <c r="G14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14">
+        <v>223</v>
+      </c>
+      <c r="I14" t="s">
+        <v>2</v>
+      </c>
+      <c r="L14">
+        <v>150025</v>
+      </c>
+      <c r="M14" t="s">
         <v>3</v>
       </c>
-      <c r="C10" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10">
-        <v>56148</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10">
-        <v>116676</v>
-      </c>
-      <c r="G10" t="s">
-        <v>69</v>
-      </c>
-      <c r="H10">
-        <v>114</v>
-      </c>
-      <c r="I10" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" t="s">
-        <v>88</v>
-      </c>
-      <c r="K10">
-        <v>40406</v>
-      </c>
-      <c r="L10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A11">
-        <v>571816</v>
-      </c>
-      <c r="B11">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
-        <v>80</v>
-      </c>
-      <c r="D11">
-        <v>36847</v>
-      </c>
-      <c r="E11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>81736</v>
-      </c>
-      <c r="G11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>223</v>
-      </c>
-      <c r="I11" t="s">
-        <v>2</v>
-      </c>
-      <c r="K11">
-        <v>38739</v>
-      </c>
-      <c r="L11" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A12">
-        <v>571816</v>
-      </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
-        <v>80</v>
-      </c>
-      <c r="D12">
-        <v>37669</v>
-      </c>
-      <c r="E12" t="s">
-        <v>175</v>
-      </c>
-      <c r="F12">
-        <v>137918</v>
-      </c>
-      <c r="G12" t="s">
-        <v>162</v>
-      </c>
-      <c r="H12">
-        <v>1181</v>
-      </c>
-      <c r="I12" t="s">
-        <v>157</v>
-      </c>
-      <c r="K12">
-        <v>22011</v>
-      </c>
-      <c r="L12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A13">
-        <v>571817</v>
-      </c>
-      <c r="B13">
-        <v>4</v>
-      </c>
-      <c r="C13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D13">
-        <v>56148</v>
-      </c>
-      <c r="E13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13">
-        <v>116676</v>
-      </c>
-      <c r="G13" t="s">
-        <v>69</v>
-      </c>
-      <c r="H13">
-        <v>114</v>
-      </c>
-      <c r="I13" t="s">
-        <v>10</v>
-      </c>
-      <c r="K13">
-        <v>124198</v>
-      </c>
-      <c r="L13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A14">
-        <v>571817</v>
-      </c>
-      <c r="B14">
-        <v>4</v>
-      </c>
-      <c r="C14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D14">
-        <v>40202</v>
-      </c>
-      <c r="E14" t="s">
-        <v>76</v>
-      </c>
-      <c r="F14">
-        <v>130214</v>
-      </c>
-      <c r="G14" t="s">
-        <v>71</v>
-      </c>
-      <c r="H14">
-        <v>875</v>
-      </c>
-      <c r="I14" t="s">
-        <v>38</v>
-      </c>
-      <c r="J14" t="s">
-        <v>89</v>
-      </c>
-      <c r="K14">
-        <v>51513</v>
-      </c>
-      <c r="L14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.45">
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A15">
-        <v>571817</v>
+        <v>571819</v>
       </c>
       <c r="B15">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D15">
-        <v>54412</v>
+        <v>40552</v>
       </c>
       <c r="E15" t="s">
-        <v>75</v>
+        <v>12</v>
       </c>
       <c r="F15">
-        <v>51273</v>
+        <v>106742</v>
       </c>
       <c r="G15" t="s">
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="H15">
-        <v>579</v>
+        <v>869</v>
       </c>
       <c r="I15" t="s">
-        <v>64</v>
-      </c>
-      <c r="J15" t="s">
-        <v>189</v>
-      </c>
-      <c r="K15">
-        <v>128692</v>
-      </c>
-      <c r="L15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.45">
+        <v>14</v>
+      </c>
+      <c r="L15">
+        <v>145535</v>
+      </c>
+      <c r="M15" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>571818</v>
       </c>
@@ -1854,14 +1923,14 @@
       <c r="I16" t="s">
         <v>14</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>120827</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>571818</v>
       </c>
@@ -1872,31 +1941,34 @@
         <v>82</v>
       </c>
       <c r="D17">
-        <v>56148</v>
+        <v>53415</v>
       </c>
       <c r="E17" t="s">
-        <v>9</v>
+        <v>180</v>
       </c>
       <c r="F17">
-        <v>116676</v>
+        <v>146271</v>
       </c>
       <c r="G17" t="s">
-        <v>69</v>
+        <v>169</v>
       </c>
       <c r="H17">
-        <v>223</v>
+        <v>1181</v>
       </c>
       <c r="I17" t="s">
-        <v>2</v>
-      </c>
-      <c r="K17">
-        <v>69830</v>
-      </c>
-      <c r="L17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+        <v>157</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="L17">
+        <v>128776</v>
+      </c>
+      <c r="M17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>571818</v>
       </c>
@@ -1907,104 +1979,104 @@
         <v>82</v>
       </c>
       <c r="D18">
-        <v>40202</v>
+        <v>53415</v>
       </c>
       <c r="E18" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="F18">
-        <v>130214</v>
+        <v>146271</v>
       </c>
       <c r="G18" t="s">
-        <v>71</v>
+        <v>169</v>
       </c>
       <c r="H18">
-        <v>579</v>
+        <v>1181</v>
       </c>
       <c r="I18" t="s">
-        <v>64</v>
-      </c>
-      <c r="J18" t="s">
-        <v>90</v>
-      </c>
-      <c r="K18">
-        <v>105241</v>
-      </c>
-      <c r="L18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+        <v>157</v>
+      </c>
+      <c r="L18">
+        <v>107006</v>
+      </c>
+      <c r="M18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19">
-        <v>571818</v>
+        <v>571816</v>
       </c>
       <c r="B19">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D19">
-        <v>40552</v>
+        <v>56148</v>
       </c>
       <c r="E19" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F19">
-        <v>133740</v>
+        <v>116676</v>
       </c>
       <c r="G19" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="H19">
-        <v>223</v>
+        <v>114</v>
       </c>
       <c r="I19" t="s">
-        <v>2</v>
-      </c>
-      <c r="K19">
-        <v>150025</v>
-      </c>
-      <c r="L19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L19">
+        <v>40406</v>
+      </c>
+      <c r="M19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>571816</v>
+      </c>
+      <c r="B20">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A20">
-        <v>571818</v>
-      </c>
-      <c r="B20">
-        <v>5</v>
-      </c>
       <c r="C20" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D20">
-        <v>36847</v>
+        <v>37669</v>
       </c>
       <c r="E20" t="s">
-        <v>0</v>
+        <v>175</v>
       </c>
       <c r="F20">
-        <v>81736</v>
+        <v>137918</v>
       </c>
       <c r="G20" t="s">
-        <v>1</v>
+        <v>162</v>
       </c>
       <c r="H20">
-        <v>223</v>
+        <v>1181</v>
       </c>
       <c r="I20" t="s">
-        <v>2</v>
-      </c>
-      <c r="K20">
-        <v>119893</v>
-      </c>
-      <c r="L20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+        <v>157</v>
+      </c>
+      <c r="L20">
+        <v>22011</v>
+      </c>
+      <c r="M20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>571818</v>
       </c>
@@ -2015,77 +2087,77 @@
         <v>82</v>
       </c>
       <c r="D21">
-        <v>36847</v>
+        <v>18663</v>
       </c>
       <c r="E21" t="s">
-        <v>0</v>
+        <v>178</v>
       </c>
       <c r="F21">
-        <v>102597</v>
+        <v>126798</v>
       </c>
       <c r="G21" t="s">
-        <v>42</v>
+        <v>167</v>
       </c>
       <c r="H21">
-        <v>223</v>
+        <v>594</v>
       </c>
       <c r="I21" t="s">
-        <v>2</v>
-      </c>
-      <c r="K21">
-        <v>109403</v>
-      </c>
-      <c r="L21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+        <v>159</v>
+      </c>
+      <c r="L21">
+        <v>164002</v>
+      </c>
+      <c r="M21" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22">
-        <v>571818</v>
+        <v>571817</v>
       </c>
       <c r="B22">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D22">
-        <v>36847</v>
+        <v>40202</v>
       </c>
       <c r="E22" t="s">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="F22">
-        <v>102597</v>
+        <v>130214</v>
       </c>
       <c r="G22" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="H22">
-        <v>223</v>
+        <v>875</v>
       </c>
       <c r="I22" t="s">
-        <v>2</v>
-      </c>
-      <c r="J22" t="s">
-        <v>91</v>
-      </c>
-      <c r="K22">
-        <v>149851</v>
-      </c>
-      <c r="L22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="L22">
+        <v>51513</v>
+      </c>
+      <c r="M22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23">
-        <v>571818</v>
+        <v>571816</v>
       </c>
       <c r="B23">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D23">
         <v>36847</v>
@@ -2094,10 +2166,10 @@
         <v>0</v>
       </c>
       <c r="F23">
-        <v>93110</v>
+        <v>81736</v>
       </c>
       <c r="G23" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="H23">
         <v>223</v>
@@ -2105,25 +2177,22 @@
       <c r="I23" t="s">
         <v>2</v>
       </c>
-      <c r="J23" t="s">
-        <v>92</v>
-      </c>
-      <c r="K23">
-        <v>101407</v>
-      </c>
-      <c r="L23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L23">
+        <v>38739</v>
+      </c>
+      <c r="M23" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24">
-        <v>571818</v>
+        <v>571819</v>
       </c>
       <c r="B24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D24">
         <v>36847</v>
@@ -2132,10 +2201,10 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>81736</v>
+        <v>93110</v>
       </c>
       <c r="G24" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="H24">
         <v>223</v>
@@ -2143,17 +2212,14 @@
       <c r="I24" t="s">
         <v>2</v>
       </c>
-      <c r="J24" t="s">
-        <v>93</v>
-      </c>
-      <c r="K24">
-        <v>74165</v>
-      </c>
-      <c r="L24" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L24">
+        <v>145224</v>
+      </c>
+      <c r="M24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>571818</v>
       </c>
@@ -2170,10 +2236,10 @@
         <v>0</v>
       </c>
       <c r="F25">
-        <v>81736</v>
+        <v>102597</v>
       </c>
       <c r="G25" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="H25">
         <v>223</v>
@@ -2181,236 +2247,234 @@
       <c r="I25" t="s">
         <v>2</v>
       </c>
-      <c r="K25">
-        <v>129881</v>
-      </c>
-      <c r="L25" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L25">
+        <v>109403</v>
+      </c>
+      <c r="M25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26">
+        <v>571816</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26">
+        <v>69289</v>
+      </c>
+      <c r="E26" t="s">
+        <v>74</v>
+      </c>
+      <c r="F26">
+        <v>126785</v>
+      </c>
+      <c r="G26" t="s">
+        <v>68</v>
+      </c>
+      <c r="H26">
+        <v>609</v>
+      </c>
+      <c r="I26" t="s">
+        <v>63</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="L26">
+        <v>35251</v>
+      </c>
+      <c r="M26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>571819</v>
+      </c>
+      <c r="B27">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27">
+        <v>107813</v>
+      </c>
+      <c r="E27" t="s">
+        <v>182</v>
+      </c>
+      <c r="F27">
+        <v>36020</v>
+      </c>
+      <c r="G27" t="s">
+        <v>172</v>
+      </c>
+      <c r="H27">
+        <v>589</v>
+      </c>
+      <c r="I27" t="s">
+        <v>160</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="L27">
+        <v>116705</v>
+      </c>
+      <c r="M27" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>571819</v>
+      </c>
+      <c r="B28">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>83</v>
+      </c>
+      <c r="D28">
+        <v>107813</v>
+      </c>
+      <c r="E28" t="s">
+        <v>182</v>
+      </c>
+      <c r="F28">
+        <v>36020</v>
+      </c>
+      <c r="G28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H28">
+        <v>589</v>
+      </c>
+      <c r="I28" t="s">
+        <v>160</v>
+      </c>
+      <c r="L28">
+        <v>164029</v>
+      </c>
+      <c r="M28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="1">
         <v>571818</v>
       </c>
-      <c r="B26">
+      <c r="B29" s="1">
         <v>5</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C29" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D26">
-        <v>39883</v>
-      </c>
-      <c r="E26" t="s">
-        <v>176</v>
-      </c>
-      <c r="F26">
-        <v>139483</v>
-      </c>
-      <c r="G26" t="s">
-        <v>163</v>
-      </c>
-      <c r="H26">
-        <v>1198</v>
-      </c>
-      <c r="I26" t="s">
-        <v>158</v>
-      </c>
-      <c r="J26" t="s">
-        <v>190</v>
-      </c>
-      <c r="K26">
-        <v>134138</v>
-      </c>
-      <c r="L26" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A27">
-        <v>571818</v>
-      </c>
-      <c r="B27">
-        <v>5</v>
-      </c>
-      <c r="C27" t="s">
-        <v>82</v>
-      </c>
-      <c r="D27">
-        <v>39883</v>
-      </c>
-      <c r="E27" t="s">
-        <v>176</v>
-      </c>
-      <c r="F27">
-        <v>139483</v>
-      </c>
-      <c r="G27" t="s">
-        <v>163</v>
-      </c>
-      <c r="H27">
-        <v>1198</v>
-      </c>
-      <c r="I27" t="s">
-        <v>158</v>
-      </c>
-      <c r="J27" t="s">
-        <v>190</v>
-      </c>
-      <c r="K27">
-        <v>108087</v>
-      </c>
-      <c r="L27" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A28">
-        <v>571818</v>
-      </c>
-      <c r="B28">
-        <v>5</v>
-      </c>
-      <c r="C28" t="s">
-        <v>82</v>
-      </c>
-      <c r="D28">
-        <v>40552</v>
-      </c>
-      <c r="E28" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28">
-        <v>133740</v>
-      </c>
-      <c r="G28" t="s">
-        <v>13</v>
-      </c>
-      <c r="H28">
-        <v>1198</v>
-      </c>
-      <c r="I28" t="s">
-        <v>158</v>
-      </c>
-      <c r="J28" t="s">
-        <v>191</v>
-      </c>
-      <c r="K28">
-        <v>107961</v>
-      </c>
-      <c r="L28" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A29">
-        <v>571818</v>
-      </c>
-      <c r="B29">
-        <v>5</v>
-      </c>
-      <c r="C29" t="s">
-        <v>82</v>
-      </c>
-      <c r="D29">
-        <v>18663</v>
-      </c>
-      <c r="E29" t="s">
-        <v>178</v>
-      </c>
-      <c r="F29">
-        <v>126798</v>
-      </c>
-      <c r="G29" t="s">
-        <v>167</v>
-      </c>
-      <c r="H29">
-        <v>594</v>
-      </c>
-      <c r="I29" t="s">
-        <v>159</v>
-      </c>
-      <c r="K29">
-        <v>164002</v>
-      </c>
-      <c r="L29" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="D29" s="1">
+        <v>27704</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F29" s="1">
+        <v>62424</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H29" s="1">
+        <v>589</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J29" s="3"/>
+      <c r="L29" s="1">
+        <v>141796</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A30">
-        <v>571818</v>
+        <v>571817</v>
       </c>
       <c r="B30">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D30">
-        <v>40552</v>
+        <v>54412</v>
       </c>
       <c r="E30" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="F30">
-        <v>133740</v>
+        <v>51273</v>
       </c>
       <c r="G30" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="H30">
-        <v>869</v>
+        <v>579</v>
       </c>
       <c r="I30" t="s">
-        <v>14</v>
-      </c>
-      <c r="J30" t="s">
-        <v>192</v>
-      </c>
-      <c r="K30">
-        <v>162160</v>
-      </c>
-      <c r="L30" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="1">
-        <v>571818</v>
-      </c>
-      <c r="B31" s="1">
-        <v>5</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D31" s="1">
-        <v>27704</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="F31" s="1">
-        <v>62424</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="H31" s="1">
-        <v>589</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="K31" s="1">
-        <v>141796</v>
-      </c>
-      <c r="L31" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
+        <v>64</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="L30">
+        <v>128692</v>
+      </c>
+      <c r="M30" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>571817</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31">
+        <v>56148</v>
+      </c>
+      <c r="E31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31">
+        <v>116676</v>
+      </c>
+      <c r="G31" t="s">
+        <v>69</v>
+      </c>
+      <c r="H31">
+        <v>114</v>
+      </c>
+      <c r="I31" t="s">
+        <v>10</v>
+      </c>
+      <c r="L31">
+        <v>124198</v>
+      </c>
+      <c r="M31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>571818</v>
       </c>
@@ -2421,31 +2485,31 @@
         <v>82</v>
       </c>
       <c r="D32">
-        <v>18663</v>
+        <v>56148</v>
       </c>
       <c r="E32" t="s">
-        <v>178</v>
+        <v>9</v>
       </c>
       <c r="F32">
-        <v>126798</v>
+        <v>116676</v>
       </c>
       <c r="G32" t="s">
-        <v>167</v>
+        <v>69</v>
       </c>
       <c r="H32">
-        <v>594</v>
+        <v>223</v>
       </c>
       <c r="I32" t="s">
-        <v>159</v>
-      </c>
-      <c r="K32">
-        <v>152057</v>
-      </c>
-      <c r="L32" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+      <c r="L32">
+        <v>69830</v>
+      </c>
+      <c r="M32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>571818</v>
       </c>
@@ -2456,34 +2520,34 @@
         <v>82</v>
       </c>
       <c r="D33">
-        <v>53415</v>
+        <v>40202</v>
       </c>
       <c r="E33" t="s">
-        <v>180</v>
+        <v>76</v>
       </c>
       <c r="F33">
-        <v>146271</v>
+        <v>130214</v>
       </c>
       <c r="G33" t="s">
-        <v>169</v>
+        <v>71</v>
       </c>
       <c r="H33">
-        <v>1181</v>
+        <v>579</v>
       </c>
       <c r="I33" t="s">
-        <v>157</v>
-      </c>
-      <c r="J33" t="s">
-        <v>193</v>
-      </c>
-      <c r="K33">
-        <v>128776</v>
-      </c>
-      <c r="L33" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
+        <v>64</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L33">
+        <v>105241</v>
+      </c>
+      <c r="M33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>571818</v>
       </c>
@@ -2494,31 +2558,31 @@
         <v>82</v>
       </c>
       <c r="D34">
-        <v>53415</v>
+        <v>36847</v>
       </c>
       <c r="E34" t="s">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="F34">
-        <v>146271</v>
+        <v>81736</v>
       </c>
       <c r="G34" t="s">
-        <v>169</v>
+        <v>1</v>
       </c>
       <c r="H34">
-        <v>1181</v>
+        <v>223</v>
       </c>
       <c r="I34" t="s">
-        <v>157</v>
-      </c>
-      <c r="K34">
-        <v>107006</v>
-      </c>
-      <c r="L34" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+      <c r="L34">
+        <v>119893</v>
+      </c>
+      <c r="M34" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>571818</v>
       </c>
@@ -2529,34 +2593,34 @@
         <v>82</v>
       </c>
       <c r="D35">
-        <v>59650</v>
+        <v>36847</v>
       </c>
       <c r="E35" t="s">
-        <v>181</v>
+        <v>0</v>
       </c>
       <c r="F35">
-        <v>81536</v>
+        <v>102597</v>
       </c>
       <c r="G35" t="s">
-        <v>170</v>
+        <v>42</v>
       </c>
       <c r="H35">
-        <v>609</v>
+        <v>223</v>
       </c>
       <c r="I35" t="s">
-        <v>63</v>
-      </c>
-      <c r="J35" t="s">
-        <v>194</v>
-      </c>
-      <c r="K35">
-        <v>60750</v>
-      </c>
-      <c r="L35" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L35">
+        <v>149851</v>
+      </c>
+      <c r="M35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>571818</v>
       </c>
@@ -2567,51 +2631,54 @@
         <v>82</v>
       </c>
       <c r="D36">
-        <v>40552</v>
+        <v>36847</v>
       </c>
       <c r="E36" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F36">
-        <v>106742</v>
+        <v>81736</v>
       </c>
       <c r="G36" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="H36">
-        <v>869</v>
+        <v>223</v>
       </c>
       <c r="I36" t="s">
-        <v>14</v>
-      </c>
-      <c r="K36">
-        <v>106236</v>
-      </c>
-      <c r="L36" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="L36">
+        <v>74165</v>
+      </c>
+      <c r="M36" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A37">
-        <v>571819</v>
+        <v>571818</v>
       </c>
       <c r="B37">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D37">
-        <v>40552</v>
+        <v>36847</v>
       </c>
       <c r="E37" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F37">
-        <v>133740</v>
+        <v>81736</v>
       </c>
       <c r="G37" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="H37">
         <v>223</v>
@@ -2619,25 +2686,22 @@
       <c r="I37" t="s">
         <v>2</v>
       </c>
-      <c r="J37" t="s">
-        <v>94</v>
-      </c>
-      <c r="K37">
-        <v>150091</v>
-      </c>
-      <c r="L37" t="s">
+      <c r="L37">
+        <v>129881</v>
+      </c>
+      <c r="M37" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>571818</v>
+      </c>
+      <c r="B38">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A38">
-        <v>571819</v>
-      </c>
-      <c r="B38">
-        <v>6</v>
-      </c>
       <c r="C38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D38">
         <v>40552</v>
@@ -2646,136 +2710,136 @@
         <v>12</v>
       </c>
       <c r="F38">
+        <v>133740</v>
+      </c>
+      <c r="G38" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38">
+        <v>1198</v>
+      </c>
+      <c r="I38" t="s">
+        <v>158</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="L38">
+        <v>107961</v>
+      </c>
+      <c r="M38" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>571818</v>
+      </c>
+      <c r="B39">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39">
+        <v>40552</v>
+      </c>
+      <c r="E39" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39">
+        <v>133740</v>
+      </c>
+      <c r="G39" t="s">
+        <v>13</v>
+      </c>
+      <c r="H39">
+        <v>869</v>
+      </c>
+      <c r="I39" t="s">
+        <v>14</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="L39">
+        <v>162160</v>
+      </c>
+      <c r="M39" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>571818</v>
+      </c>
+      <c r="B40">
+        <v>5</v>
+      </c>
+      <c r="C40" t="s">
+        <v>82</v>
+      </c>
+      <c r="D40">
+        <v>18663</v>
+      </c>
+      <c r="E40" t="s">
+        <v>178</v>
+      </c>
+      <c r="F40">
+        <v>126798</v>
+      </c>
+      <c r="G40" t="s">
+        <v>167</v>
+      </c>
+      <c r="H40">
+        <v>594</v>
+      </c>
+      <c r="I40" t="s">
+        <v>159</v>
+      </c>
+      <c r="L40">
+        <v>152057</v>
+      </c>
+      <c r="M40" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>571818</v>
+      </c>
+      <c r="B41">
+        <v>5</v>
+      </c>
+      <c r="C41" t="s">
+        <v>82</v>
+      </c>
+      <c r="D41">
+        <v>40552</v>
+      </c>
+      <c r="E41" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41">
         <v>106742</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G41" t="s">
         <v>16</v>
       </c>
-      <c r="H38">
-        <v>223</v>
-      </c>
-      <c r="I38" t="s">
-        <v>2</v>
-      </c>
-      <c r="J38" t="s">
-        <v>95</v>
-      </c>
-      <c r="K38">
-        <v>134608</v>
-      </c>
-      <c r="L38" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A39">
-        <v>571819</v>
-      </c>
-      <c r="B39">
-        <v>6</v>
-      </c>
-      <c r="C39" t="s">
-        <v>83</v>
-      </c>
-      <c r="D39">
-        <v>69289</v>
-      </c>
-      <c r="E39" t="s">
-        <v>74</v>
-      </c>
-      <c r="F39">
-        <v>126785</v>
-      </c>
-      <c r="G39" t="s">
-        <v>68</v>
-      </c>
-      <c r="H39">
-        <v>609</v>
-      </c>
-      <c r="I39" t="s">
-        <v>63</v>
-      </c>
-      <c r="J39" t="s">
-        <v>96</v>
-      </c>
-      <c r="K39">
-        <v>131893</v>
-      </c>
-      <c r="L39" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A40">
-        <v>571819</v>
-      </c>
-      <c r="B40">
-        <v>6</v>
-      </c>
-      <c r="C40" t="s">
-        <v>83</v>
-      </c>
-      <c r="D40">
-        <v>36847</v>
-      </c>
-      <c r="E40" t="s">
-        <v>0</v>
-      </c>
-      <c r="F40">
-        <v>102597</v>
-      </c>
-      <c r="G40" t="s">
-        <v>42</v>
-      </c>
-      <c r="H40">
-        <v>223</v>
-      </c>
-      <c r="I40" t="s">
-        <v>2</v>
-      </c>
-      <c r="K40">
-        <v>155140</v>
-      </c>
-      <c r="L40" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A41">
-        <v>571819</v>
-      </c>
-      <c r="B41">
-        <v>6</v>
-      </c>
-      <c r="C41" t="s">
-        <v>83</v>
-      </c>
-      <c r="D41">
-        <v>36847</v>
-      </c>
-      <c r="E41" t="s">
-        <v>0</v>
-      </c>
-      <c r="F41">
-        <v>102597</v>
-      </c>
-      <c r="G41" t="s">
-        <v>42</v>
-      </c>
       <c r="H41">
-        <v>223</v>
+        <v>869</v>
       </c>
       <c r="I41" t="s">
-        <v>2</v>
-      </c>
-      <c r="K41">
-        <v>169475</v>
-      </c>
-      <c r="L41" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.45">
+        <v>14</v>
+      </c>
+      <c r="L41">
+        <v>106236</v>
+      </c>
+      <c r="M41" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>571819</v>
       </c>
@@ -2786,16 +2850,16 @@
         <v>83</v>
       </c>
       <c r="D42">
-        <v>36847</v>
+        <v>40552</v>
       </c>
       <c r="E42" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F42">
-        <v>93110</v>
+        <v>133740</v>
       </c>
       <c r="G42" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H42">
         <v>223</v>
@@ -2803,14 +2867,17 @@
       <c r="I42" t="s">
         <v>2</v>
       </c>
-      <c r="K42">
-        <v>145224</v>
-      </c>
-      <c r="L42" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="J42" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="L42">
+        <v>150091</v>
+      </c>
+      <c r="M42" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>571819</v>
       </c>
@@ -2821,34 +2888,34 @@
         <v>83</v>
       </c>
       <c r="D43">
-        <v>39883</v>
+        <v>40552</v>
       </c>
       <c r="E43" t="s">
-        <v>176</v>
+        <v>12</v>
       </c>
       <c r="F43">
-        <v>44643</v>
+        <v>106742</v>
       </c>
       <c r="G43" t="s">
-        <v>171</v>
+        <v>16</v>
       </c>
       <c r="H43">
-        <v>1198</v>
+        <v>223</v>
       </c>
       <c r="I43" t="s">
-        <v>158</v>
-      </c>
-      <c r="J43" t="s">
-        <v>195</v>
-      </c>
-      <c r="K43">
-        <v>129688</v>
-      </c>
-      <c r="L43" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="L43">
+        <v>134608</v>
+      </c>
+      <c r="M43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>571819</v>
       </c>
@@ -2859,34 +2926,34 @@
         <v>83</v>
       </c>
       <c r="D44">
-        <v>39883</v>
+        <v>69289</v>
       </c>
       <c r="E44" t="s">
-        <v>176</v>
+        <v>74</v>
       </c>
       <c r="F44">
-        <v>44643</v>
+        <v>126785</v>
       </c>
       <c r="G44" t="s">
-        <v>171</v>
+        <v>68</v>
       </c>
       <c r="H44">
-        <v>1198</v>
+        <v>609</v>
       </c>
       <c r="I44" t="s">
-        <v>158</v>
-      </c>
-      <c r="J44" t="s">
-        <v>195</v>
-      </c>
-      <c r="K44">
-        <v>129079</v>
-      </c>
-      <c r="L44" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.45">
+        <v>63</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="L44">
+        <v>131893</v>
+      </c>
+      <c r="M44" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>571819</v>
       </c>
@@ -2897,31 +2964,31 @@
         <v>83</v>
       </c>
       <c r="D45">
-        <v>18663</v>
+        <v>36847</v>
       </c>
       <c r="E45" t="s">
-        <v>178</v>
+        <v>0</v>
       </c>
       <c r="F45">
-        <v>126798</v>
+        <v>102597</v>
       </c>
       <c r="G45" t="s">
-        <v>167</v>
+        <v>42</v>
       </c>
       <c r="H45">
-        <v>594</v>
+        <v>223</v>
       </c>
       <c r="I45" t="s">
-        <v>159</v>
-      </c>
-      <c r="K45">
-        <v>151413</v>
-      </c>
-      <c r="L45" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+      <c r="L45">
+        <v>155140</v>
+      </c>
+      <c r="M45" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>571819</v>
       </c>
@@ -2938,10 +3005,10 @@
         <v>0</v>
       </c>
       <c r="F46">
-        <v>93110</v>
+        <v>102597</v>
       </c>
       <c r="G46" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="H46">
         <v>223</v>
@@ -2949,14 +3016,14 @@
       <c r="I46" t="s">
         <v>2</v>
       </c>
-      <c r="K46">
-        <v>101580</v>
-      </c>
-      <c r="L46" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L46">
+        <v>169475</v>
+      </c>
+      <c r="M46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>571819</v>
       </c>
@@ -2967,31 +3034,31 @@
         <v>83</v>
       </c>
       <c r="D47">
-        <v>107813</v>
+        <v>18663</v>
       </c>
       <c r="E47" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="F47">
-        <v>36020</v>
+        <v>126798</v>
       </c>
       <c r="G47" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="H47">
-        <v>589</v>
+        <v>594</v>
       </c>
       <c r="I47" t="s">
-        <v>160</v>
-      </c>
-      <c r="K47">
-        <v>164029</v>
-      </c>
-      <c r="L47" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.45">
+        <v>159</v>
+      </c>
+      <c r="L47">
+        <v>151413</v>
+      </c>
+      <c r="M47" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>571819</v>
       </c>
@@ -3019,14 +3086,14 @@
       <c r="I48" t="s">
         <v>2</v>
       </c>
-      <c r="K48">
-        <v>145200</v>
-      </c>
-      <c r="L48" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="L48">
+        <v>101580</v>
+      </c>
+      <c r="M48" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>571819</v>
       </c>
@@ -3037,34 +3104,31 @@
         <v>83</v>
       </c>
       <c r="D49">
-        <v>107813</v>
+        <v>36847</v>
       </c>
       <c r="E49" t="s">
-        <v>182</v>
+        <v>0</v>
       </c>
       <c r="F49">
-        <v>36020</v>
+        <v>93110</v>
       </c>
       <c r="G49" t="s">
-        <v>172</v>
+        <v>17</v>
       </c>
       <c r="H49">
-        <v>589</v>
+        <v>223</v>
       </c>
       <c r="I49" t="s">
-        <v>160</v>
-      </c>
-      <c r="J49" t="s">
-        <v>196</v>
-      </c>
-      <c r="K49">
-        <v>116705</v>
-      </c>
-      <c r="L49" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+      <c r="L49">
+        <v>145200</v>
+      </c>
+      <c r="M49" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>571819</v>
       </c>
@@ -3092,57 +3156,93 @@
       <c r="I50" t="s">
         <v>66</v>
       </c>
-      <c r="K50">
+      <c r="L50">
         <v>120917</v>
       </c>
-      <c r="L50" t="s">
+      <c r="M50" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A51">
-        <v>571825</v>
+        <v>571827</v>
       </c>
       <c r="B51">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C51" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D51">
-        <v>40552</v>
+        <v>53869</v>
       </c>
       <c r="E51" t="s">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="F51">
-        <v>106742</v>
+        <v>145220</v>
       </c>
       <c r="G51" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="H51">
-        <v>869</v>
+        <v>628</v>
       </c>
       <c r="I51" t="s">
-        <v>14</v>
-      </c>
-      <c r="K51">
-        <v>145535</v>
-      </c>
-      <c r="L51" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.45">
+        <v>66</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="K51" t="s">
+        <v>212</v>
+      </c>
+      <c r="L51">
+        <v>179705</v>
+      </c>
+      <c r="M51" t="s">
+        <v>56</v>
+      </c>
+      <c r="N51">
+        <v>152452</v>
+      </c>
+      <c r="O51" t="s">
+        <v>57</v>
+      </c>
+      <c r="P51">
+        <v>172811</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>58</v>
+      </c>
+      <c r="R51">
+        <v>172810</v>
+      </c>
+      <c r="S51" t="s">
+        <v>60</v>
+      </c>
+      <c r="T51">
+        <v>172812</v>
+      </c>
+      <c r="U51" t="s">
+        <v>61</v>
+      </c>
+      <c r="V51">
+        <v>172809</v>
+      </c>
+      <c r="W51" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A52">
-        <v>571827</v>
+        <v>571828</v>
       </c>
       <c r="B52">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C52" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D52">
         <v>53869</v>
@@ -3162,47 +3262,14 @@
       <c r="I52" t="s">
         <v>66</v>
       </c>
-      <c r="J52" t="s">
-        <v>97</v>
-      </c>
-      <c r="K52">
-        <v>179705</v>
-      </c>
-      <c r="L52" t="s">
-        <v>56</v>
-      </c>
-      <c r="M52">
-        <v>152452</v>
-      </c>
-      <c r="N52" t="s">
-        <v>57</v>
-      </c>
-      <c r="O52">
-        <v>172811</v>
-      </c>
-      <c r="P52" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q52">
-        <v>172809</v>
-      </c>
-      <c r="R52" t="s">
-        <v>59</v>
-      </c>
-      <c r="S52">
-        <v>172810</v>
-      </c>
-      <c r="T52" t="s">
-        <v>60</v>
-      </c>
-      <c r="U52">
-        <v>172812</v>
-      </c>
-      <c r="V52" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="L52">
+        <v>123786</v>
+      </c>
+      <c r="M52" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>571828</v>
       </c>
@@ -3213,51 +3280,51 @@
         <v>31</v>
       </c>
       <c r="D53">
-        <v>53869</v>
+        <v>18663</v>
       </c>
       <c r="E53" t="s">
-        <v>77</v>
+        <v>178</v>
       </c>
       <c r="F53">
-        <v>145220</v>
+        <v>126798</v>
       </c>
       <c r="G53" t="s">
-        <v>72</v>
+        <v>167</v>
       </c>
       <c r="H53">
-        <v>628</v>
+        <v>594</v>
       </c>
       <c r="I53" t="s">
-        <v>66</v>
-      </c>
-      <c r="K53">
-        <v>123786</v>
-      </c>
-      <c r="L53" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.45">
+        <v>159</v>
+      </c>
+      <c r="L53">
+        <v>130283</v>
+      </c>
+      <c r="M53" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A54">
-        <v>571828</v>
+        <v>571830</v>
       </c>
       <c r="B54">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C54" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D54">
-        <v>18663</v>
+        <v>103897</v>
       </c>
       <c r="E54" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="F54">
-        <v>126798</v>
+        <v>166762</v>
       </c>
       <c r="G54" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="H54">
         <v>594</v>
@@ -3265,22 +3332,49 @@
       <c r="I54" t="s">
         <v>159</v>
       </c>
-      <c r="K54">
-        <v>130283</v>
-      </c>
-      <c r="L54" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="J54" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="L54">
+        <v>177919</v>
+      </c>
+      <c r="M54" t="s">
+        <v>144</v>
+      </c>
+      <c r="N54">
+        <v>172972</v>
+      </c>
+      <c r="O54" t="s">
+        <v>145</v>
+      </c>
+      <c r="P54">
+        <v>164338</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>146</v>
+      </c>
+      <c r="R54">
+        <v>172339</v>
+      </c>
+      <c r="S54" t="s">
+        <v>147</v>
+      </c>
+      <c r="T54">
+        <v>144293</v>
+      </c>
+      <c r="U54" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A55">
-        <v>571830</v>
+        <v>571831</v>
       </c>
       <c r="B55">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C55" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D55">
         <v>103897</v>
@@ -3300,41 +3394,35 @@
       <c r="I55" t="s">
         <v>159</v>
       </c>
-      <c r="J55" t="s">
-        <v>197</v>
-      </c>
-      <c r="K55">
-        <v>177919</v>
-      </c>
-      <c r="L55" t="s">
-        <v>144</v>
-      </c>
-      <c r="M55">
-        <v>172972</v>
-      </c>
-      <c r="N55" t="s">
-        <v>145</v>
-      </c>
-      <c r="O55">
-        <v>164338</v>
-      </c>
-      <c r="P55" t="s">
-        <v>146</v>
-      </c>
-      <c r="Q55">
-        <v>172339</v>
-      </c>
-      <c r="R55" t="s">
-        <v>147</v>
-      </c>
-      <c r="S55">
-        <v>144293</v>
-      </c>
-      <c r="T55" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="J55" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="L55">
+        <v>170947</v>
+      </c>
+      <c r="M55" t="s">
+        <v>153</v>
+      </c>
+      <c r="N55">
+        <v>151103</v>
+      </c>
+      <c r="O55" t="s">
+        <v>155</v>
+      </c>
+      <c r="P55">
+        <v>171294</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>154</v>
+      </c>
+      <c r="R55">
+        <v>177921</v>
+      </c>
+      <c r="S55" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>571831</v>
       </c>
@@ -3362,82 +3450,67 @@
       <c r="I56" t="s">
         <v>65</v>
       </c>
-      <c r="K56">
+      <c r="L56">
         <v>176931</v>
       </c>
-      <c r="L56" t="s">
+      <c r="M56" t="s">
         <v>149</v>
       </c>
-      <c r="M56">
+      <c r="N56">
         <v>180169</v>
       </c>
-      <c r="N56" t="s">
+      <c r="O56" t="s">
         <v>150</v>
       </c>
-      <c r="O56">
+      <c r="P56">
         <v>159675</v>
       </c>
-      <c r="P56" t="s">
+      <c r="Q56" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A57">
-        <v>571831</v>
+        <v>571820</v>
       </c>
       <c r="B57">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C57" t="s">
-        <v>25</v>
+        <v>102</v>
       </c>
       <c r="D57">
-        <v>103897</v>
+        <v>27704</v>
       </c>
       <c r="E57" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F57">
-        <v>166762</v>
+        <v>62424</v>
       </c>
       <c r="G57" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H57">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="I57" t="s">
-        <v>159</v>
-      </c>
-      <c r="J57" t="s">
-        <v>198</v>
-      </c>
-      <c r="K57">
-        <v>177921</v>
-      </c>
-      <c r="L57" t="s">
-        <v>152</v>
-      </c>
-      <c r="M57">
-        <v>170947</v>
-      </c>
-      <c r="N57" t="s">
-        <v>153</v>
-      </c>
-      <c r="O57">
-        <v>171294</v>
-      </c>
-      <c r="P57" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q57">
-        <v>151103</v>
-      </c>
-      <c r="R57" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.45">
+        <v>160</v>
+      </c>
+      <c r="L57">
+        <v>166499</v>
+      </c>
+      <c r="M57" t="s">
+        <v>156</v>
+      </c>
+      <c r="N57">
+        <v>164029</v>
+      </c>
+      <c r="O57" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>571820</v>
       </c>
@@ -3465,61 +3538,58 @@
       <c r="I58" t="s">
         <v>65</v>
       </c>
-      <c r="J58" t="s">
+      <c r="J58" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="K58">
+      <c r="L58">
         <v>112424</v>
       </c>
-      <c r="L58" t="s">
+      <c r="M58" t="s">
         <v>99</v>
       </c>
-      <c r="M58">
+      <c r="N58">
         <v>95591</v>
       </c>
-      <c r="N58" t="s">
+      <c r="O58" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A59">
-        <v>571820</v>
+        <v>571818</v>
       </c>
       <c r="B59">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C59" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="D59">
-        <v>27704</v>
+        <v>36847</v>
       </c>
       <c r="E59" t="s">
-        <v>179</v>
+        <v>0</v>
       </c>
       <c r="F59">
-        <v>62424</v>
+        <v>93110</v>
       </c>
       <c r="G59" t="s">
-        <v>168</v>
+        <v>17</v>
       </c>
       <c r="H59">
-        <v>589</v>
+        <v>223</v>
       </c>
       <c r="I59" t="s">
-        <v>160</v>
-      </c>
-      <c r="K59">
-        <v>166499</v>
-      </c>
-      <c r="L59" t="s">
-        <v>156</v>
-      </c>
-      <c r="M59">
-        <v>164029</v>
-      </c>
-      <c r="N59" t="s">
-        <v>139</v>
+        <v>2</v>
+      </c>
+      <c r="J59" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L59">
+        <v>101407</v>
+      </c>
+      <c r="M59" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -3529,19 +3599,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA9D28CB-C6E2-4B8D-9091-1FD20615DBE1}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="3" max="3" width="45" customWidth="1"/>
+    <col min="5" max="5" width="26.06640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1">
         <v>571814</v>
       </c>
@@ -3554,8 +3625,11 @@
       <c r="D1">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>571815</v>
       </c>
@@ -3568,8 +3642,11 @@
       <c r="D2">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>571816</v>
       </c>
@@ -3582,8 +3659,11 @@
       <c r="D3">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>571817</v>
       </c>
@@ -3596,8 +3676,11 @@
       <c r="D4">
         <v>1063</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>571818</v>
       </c>
@@ -3610,8 +3693,11 @@
       <c r="D5">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>571819</v>
       </c>
@@ -3624,8 +3710,11 @@
       <c r="D6">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>571821</v>
       </c>
@@ -3636,10 +3725,13 @@
         <v>84</v>
       </c>
       <c r="D7">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+        <v>30</v>
+      </c>
+      <c r="F7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>571822</v>
       </c>
@@ -3650,10 +3742,13 @@
         <v>8</v>
       </c>
       <c r="D8">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>571823</v>
       </c>
@@ -3664,10 +3759,13 @@
         <v>27</v>
       </c>
       <c r="D9">
-        <v>1063</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+        <v>1061</v>
+      </c>
+      <c r="F9" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>571824</v>
       </c>
@@ -3678,10 +3776,13 @@
         <v>11</v>
       </c>
       <c r="D10">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="F10" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>571825</v>
       </c>
@@ -3692,10 +3793,13 @@
         <v>22</v>
       </c>
       <c r="D11">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+      <c r="F11" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>571827</v>
       </c>
@@ -3711,8 +3815,11 @@
       <c r="E12" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F12" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>571828</v>
       </c>
@@ -3729,7 +3836,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>571829</v>
       </c>
@@ -3745,8 +3852,11 @@
       <c r="E14" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F14" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>571830</v>
       </c>
@@ -3762,8 +3872,11 @@
       <c r="E15" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>571831</v>
       </c>
@@ -3779,8 +3892,11 @@
       <c r="E16" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F16" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>571832</v>
       </c>
@@ -3797,7 +3913,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>571820</v>
       </c>
@@ -3809,6 +3925,9 @@
       </c>
       <c r="D18">
         <v>1065</v>
+      </c>
+      <c r="F18" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -4369,7 +4488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D5152B9-B788-4BDE-A1B2-C618945E4F4F}">
   <dimension ref="A1:B94"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
SM 2022 2022-07-12 Biograf bytt till charlie för Amalia Glimmerhav och Heuman bytt till Biograf
</commit_message>
<xml_diff>
--- a/mallar/import/Sm2022/extr3_sm2022.xlsx
+++ b/mallar/import/Sm2022/extr3_sm2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\episerver\voltige\VoltigeClosedXML\mallar\import\Sm2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{993390DA-541A-484A-90C2-DD432D527406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B175CF6-19E5-465C-9FB0-CB50615D5922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="8820" windowWidth="29040" windowHeight="17640" tabRatio="483" xr2:uid="{9C6C5895-3CBC-495A-8EC3-24DF642F0EB2}"/>
+    <workbookView xWindow="-60" yWindow="-60" windowWidth="21720" windowHeight="13020" tabRatio="483" xr2:uid="{9C6C5895-3CBC-495A-8EC3-24DF642F0EB2}"/>
   </bookViews>
   <sheets>
     <sheet name="ekipage" sheetId="1" r:id="rId1"/>
@@ -1245,8 +1245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B3B0E3-2027-4083-B582-AAB0C4C3F786}">
   <dimension ref="A1:W60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView tabSelected="1" topLeftCell="C41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1843,17 +1843,17 @@
       <c r="C9" t="s">
         <v>82</v>
       </c>
-      <c r="D9">
-        <v>59650</v>
-      </c>
-      <c r="E9" t="s">
-        <v>180</v>
-      </c>
-      <c r="F9">
-        <v>81536</v>
-      </c>
-      <c r="G9" t="s">
-        <v>169</v>
+      <c r="D9" s="6">
+        <v>18663</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="F9" s="6">
+        <v>120239</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>165</v>
       </c>
       <c r="H9">
         <v>609</v>
@@ -3442,17 +3442,17 @@
       <c r="C52" t="s">
         <v>31</v>
       </c>
-      <c r="D52">
-        <v>53869</v>
-      </c>
-      <c r="E52" t="s">
-        <v>77</v>
-      </c>
-      <c r="F52">
-        <v>145220</v>
-      </c>
-      <c r="G52" t="s">
-        <v>72</v>
+      <c r="D52" s="6">
+        <v>59650</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="F52" s="6">
+        <v>81536</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>169</v>
       </c>
       <c r="H52">
         <v>628</v>
@@ -4374,7 +4374,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="A21" sqref="A21:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
SM 2022 - efter tävling
</commit_message>
<xml_diff>
--- a/mallar/import/Sm2022/extr3_sm2022.xlsx
+++ b/mallar/import/Sm2022/extr3_sm2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\episerver\voltige\VoltigeClosedXML\mallar\import\Sm2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D67D676-847D-46B6-B4A1-EE87918792E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{155F73BB-10B1-40E5-BB35-FA55E77D56C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" tabRatio="483" xr2:uid="{9C6C5895-3CBC-495A-8EC3-24DF642F0EB2}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="276">
   <si>
     <t>Linda Jenvall</t>
   </si>
@@ -562,9 +562,6 @@
     <t>Christina Müller</t>
   </si>
   <si>
-    <t>Gabriela Persson</t>
-  </si>
-  <si>
     <t>Anna Andersson</t>
   </si>
   <si>
@@ -863,6 +860,12 @@
   </si>
   <si>
     <t>Pas de Deux SM</t>
+  </si>
+  <si>
+    <t>Freilene_Fifija</t>
+  </si>
+  <si>
+    <t>Ronja Persson</t>
   </si>
 </sst>
 </file>
@@ -1243,7 +1246,7 @@
   <dimension ref="A1:W59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1294,10 +1297,10 @@
         <v>2</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L1">
         <v>115495</v>
@@ -1347,64 +1350,64 @@
         <v>78</v>
       </c>
       <c r="D2">
-        <v>53144</v>
+        <v>68838</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="F2">
-        <v>138736</v>
+        <v>7110</v>
       </c>
       <c r="G2" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="H2">
-        <v>609</v>
+        <v>875</v>
       </c>
       <c r="I2" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K2" t="s">
-        <v>269</v>
+        <v>203</v>
       </c>
       <c r="L2">
-        <v>70336</v>
+        <v>51513</v>
       </c>
       <c r="M2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="N2">
-        <v>87139</v>
+        <v>108189</v>
       </c>
       <c r="O2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="P2">
-        <v>57826</v>
+        <v>82678</v>
       </c>
       <c r="Q2" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="R2">
-        <v>34693</v>
+        <v>36794</v>
       </c>
       <c r="S2" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="T2">
-        <v>134144</v>
+        <v>105337</v>
       </c>
       <c r="U2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="V2">
-        <v>159908</v>
+        <v>164089</v>
       </c>
       <c r="W2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="42.75" x14ac:dyDescent="0.45">
@@ -1418,64 +1421,64 @@
         <v>78</v>
       </c>
       <c r="D3">
-        <v>68838</v>
+        <v>53144</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="F3">
-        <v>7110</v>
+        <v>138736</v>
       </c>
       <c r="G3" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="H3">
-        <v>875</v>
+        <v>609</v>
       </c>
       <c r="I3" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K3" t="s">
-        <v>204</v>
+        <v>268</v>
       </c>
       <c r="L3">
-        <v>51513</v>
+        <v>70336</v>
       </c>
       <c r="M3" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="N3">
-        <v>108189</v>
+        <v>87139</v>
       </c>
       <c r="O3" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="P3">
-        <v>82678</v>
+        <v>57826</v>
       </c>
       <c r="Q3" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="R3">
-        <v>36794</v>
+        <v>34693</v>
       </c>
       <c r="S3" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="T3">
-        <v>105337</v>
+        <v>134144</v>
       </c>
       <c r="U3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="V3">
-        <v>164089</v>
+        <v>159908</v>
       </c>
       <c r="W3" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.45">
@@ -1492,7 +1495,7 @@
         <v>37669</v>
       </c>
       <c r="E4" t="s">
-        <v>174</v>
+        <v>275</v>
       </c>
       <c r="F4">
         <v>137918</v>
@@ -1507,7 +1510,7 @@
         <v>156</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="L4">
         <v>22011</v>
@@ -1546,7 +1549,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:23" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>571815</v>
       </c>
@@ -1557,64 +1560,64 @@
         <v>79</v>
       </c>
       <c r="D5">
-        <v>39883</v>
+        <v>68838</v>
       </c>
       <c r="E5" t="s">
-        <v>175</v>
+        <v>40</v>
       </c>
       <c r="F5">
-        <v>139483</v>
+        <v>137228</v>
       </c>
       <c r="G5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H5">
-        <v>1198</v>
+        <v>875</v>
       </c>
       <c r="I5" t="s">
-        <v>157</v>
+        <v>38</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="K5" s="4" t="s">
-        <v>220</v>
+      <c r="K5" t="s">
+        <v>205</v>
       </c>
       <c r="L5">
-        <v>129485</v>
+        <v>107737</v>
       </c>
       <c r="M5" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="N5">
-        <v>108087</v>
+        <v>129183</v>
       </c>
       <c r="O5" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="P5">
-        <v>134138</v>
+        <v>127857</v>
       </c>
       <c r="Q5" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="R5">
-        <v>129079</v>
+        <v>120375</v>
       </c>
       <c r="S5" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="T5">
-        <v>107961</v>
+        <v>140351</v>
       </c>
       <c r="U5" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="V5">
-        <v>129688</v>
+        <v>123591</v>
       </c>
       <c r="W5" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.45">
@@ -1628,67 +1631,67 @@
         <v>79</v>
       </c>
       <c r="D6">
-        <v>18663</v>
+        <v>39883</v>
       </c>
       <c r="E6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F6">
-        <v>120239</v>
+        <v>139483</v>
       </c>
       <c r="G6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H6">
-        <v>594</v>
+        <v>1198</v>
       </c>
       <c r="I6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="L6">
-        <v>151413</v>
+        <v>129485</v>
       </c>
       <c r="M6" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="N6">
-        <v>152057</v>
+        <v>108087</v>
       </c>
       <c r="O6" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="P6">
-        <v>164002</v>
+        <v>134138</v>
       </c>
       <c r="Q6" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="R6">
-        <v>155756</v>
+        <v>129079</v>
       </c>
       <c r="S6" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="T6">
-        <v>160046</v>
+        <v>107961</v>
       </c>
       <c r="U6" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="V6">
-        <v>140835</v>
+        <v>129688</v>
       </c>
       <c r="W6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" ht="42.75" x14ac:dyDescent="0.45">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>571815</v>
       </c>
@@ -1699,102 +1702,100 @@
         <v>79</v>
       </c>
       <c r="D7">
-        <v>68838</v>
+        <v>18663</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>176</v>
       </c>
       <c r="F7">
-        <v>137228</v>
+        <v>120239</v>
       </c>
       <c r="G7" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H7">
-        <v>875</v>
+        <v>594</v>
       </c>
       <c r="I7" t="s">
-        <v>38</v>
+        <v>158</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="4" t="s">
         <v>206</v>
       </c>
       <c r="L7">
-        <v>107737</v>
+        <v>151413</v>
       </c>
       <c r="M7" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="N7">
-        <v>129183</v>
+        <v>152057</v>
       </c>
       <c r="O7" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="P7">
-        <v>127857</v>
+        <v>164002</v>
       </c>
       <c r="Q7" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="R7">
-        <v>120375</v>
+        <v>155756</v>
       </c>
       <c r="S7" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="T7">
-        <v>140351</v>
+        <v>160046</v>
       </c>
       <c r="U7" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="V7">
-        <v>123591</v>
+        <v>140835</v>
       </c>
       <c r="W7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A8">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="1">
         <v>571818</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>5</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="6">
-        <v>18663</v>
-      </c>
-      <c r="E8" s="6" t="s">
+      <c r="D8" s="1">
+        <v>27704</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="F8" s="6">
-        <v>120239</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="H8">
-        <v>609</v>
-      </c>
-      <c r="I8" t="s">
-        <v>63</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="L8">
-        <v>60750</v>
-      </c>
-      <c r="M8" t="s">
-        <v>136</v>
+      <c r="F8" s="1">
+        <v>62424</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H8" s="1">
+        <v>589</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="J8" s="3"/>
+      <c r="L8" s="1">
+        <v>141796</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.45">
@@ -1808,69 +1809,63 @@
         <v>82</v>
       </c>
       <c r="D9">
-        <v>39883</v>
+        <v>40552</v>
       </c>
       <c r="E9" t="s">
-        <v>175</v>
+        <v>12</v>
       </c>
       <c r="F9">
-        <v>139483</v>
+        <v>106742</v>
       </c>
       <c r="G9" t="s">
-        <v>162</v>
+        <v>16</v>
       </c>
       <c r="H9">
-        <v>1198</v>
+        <v>869</v>
       </c>
       <c r="I9" t="s">
-        <v>157</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>188</v>
+        <v>14</v>
       </c>
       <c r="L9">
-        <v>108087</v>
+        <v>120827</v>
       </c>
       <c r="M9" t="s">
-        <v>115</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A10">
-        <v>571818</v>
+        <v>571819</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D10">
-        <v>39883</v>
+        <v>36847</v>
       </c>
       <c r="E10" t="s">
-        <v>175</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>139483</v>
+        <v>93110</v>
       </c>
       <c r="G10" t="s">
-        <v>162</v>
+        <v>17</v>
       </c>
       <c r="H10">
-        <v>1198</v>
+        <v>223</v>
       </c>
       <c r="I10" t="s">
-        <v>157</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>188</v>
+        <v>2</v>
       </c>
       <c r="L10">
-        <v>134138</v>
+        <v>145200</v>
       </c>
       <c r="M10" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.45">
@@ -1884,51 +1879,51 @@
         <v>83</v>
       </c>
       <c r="D11">
-        <v>39883</v>
+        <v>40552</v>
       </c>
       <c r="E11" t="s">
-        <v>175</v>
-      </c>
-      <c r="F11">
-        <v>44643</v>
-      </c>
-      <c r="G11" t="s">
-        <v>170</v>
+        <v>12</v>
+      </c>
+      <c r="F11" s="6">
+        <v>99</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>274</v>
       </c>
       <c r="H11">
-        <v>628</v>
+        <v>869</v>
       </c>
       <c r="I11" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="L11">
-        <v>120917</v>
+        <v>145535</v>
       </c>
       <c r="M11" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A12">
-        <v>571819</v>
+        <v>571818</v>
       </c>
       <c r="B12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D12">
         <v>39883</v>
       </c>
       <c r="E12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F12">
-        <v>44643</v>
+        <v>139483</v>
       </c>
       <c r="G12" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="H12">
         <v>1198</v>
@@ -1937,51 +1932,51 @@
         <v>157</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="L12">
-        <v>129688</v>
+        <v>108087</v>
       </c>
       <c r="M12" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A13">
-        <v>571819</v>
+        <v>571818</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>83</v>
-      </c>
-      <c r="D13">
-        <v>39883</v>
-      </c>
-      <c r="E13" t="s">
-        <v>175</v>
-      </c>
-      <c r="F13">
-        <v>44643</v>
-      </c>
-      <c r="G13" t="s">
-        <v>170</v>
+        <v>82</v>
+      </c>
+      <c r="D13" s="6">
+        <v>18663</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="F13" s="6">
+        <v>120239</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>165</v>
       </c>
       <c r="H13">
-        <v>1198</v>
+        <v>609</v>
       </c>
       <c r="I13" t="s">
-        <v>157</v>
+        <v>63</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L13">
-        <v>129079</v>
+        <v>60750</v>
       </c>
       <c r="M13" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.45">
@@ -1995,107 +1990,107 @@
         <v>82</v>
       </c>
       <c r="D14">
-        <v>40552</v>
+        <v>53415</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>178</v>
       </c>
       <c r="F14">
-        <v>133740</v>
+        <v>146271</v>
       </c>
       <c r="G14" t="s">
-        <v>13</v>
+        <v>168</v>
       </c>
       <c r="H14">
-        <v>869</v>
+        <v>1181</v>
       </c>
       <c r="I14" t="s">
-        <v>14</v>
+        <v>156</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>190</v>
       </c>
       <c r="L14">
-        <v>162160</v>
+        <v>128776</v>
       </c>
       <c r="M14" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.45">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A15">
-        <v>571818</v>
+        <v>571819</v>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D15">
-        <v>40552</v>
+        <v>69289</v>
       </c>
       <c r="E15" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="F15">
-        <v>133740</v>
+        <v>126785</v>
       </c>
       <c r="G15" t="s">
-        <v>13</v>
+        <v>68</v>
       </c>
       <c r="H15">
-        <v>1198</v>
+        <v>609</v>
       </c>
       <c r="I15" t="s">
-        <v>157</v>
+        <v>63</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>189</v>
+        <v>95</v>
       </c>
       <c r="L15">
-        <v>107961</v>
+        <v>131893</v>
       </c>
       <c r="M15" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.45">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A16">
-        <v>571819</v>
+        <v>571817</v>
       </c>
       <c r="B16">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D16">
-        <v>40552</v>
+        <v>54412</v>
       </c>
       <c r="E16" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="F16">
-        <v>133740</v>
+        <v>51273</v>
       </c>
       <c r="G16" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="H16">
-        <v>223</v>
+        <v>579</v>
       </c>
       <c r="I16" t="s">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>93</v>
+        <v>186</v>
       </c>
       <c r="L16">
-        <v>150091</v>
+        <v>128692</v>
       </c>
       <c r="M16" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.45">
@@ -2109,16 +2104,16 @@
         <v>82</v>
       </c>
       <c r="D17">
-        <v>40552</v>
+        <v>56148</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F17">
-        <v>133740</v>
+        <v>116676</v>
       </c>
       <c r="G17" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="H17">
         <v>223</v>
@@ -2127,33 +2122,33 @@
         <v>2</v>
       </c>
       <c r="L17">
-        <v>150025</v>
+        <v>69830</v>
       </c>
       <c r="M17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18">
-        <v>571819</v>
+        <v>571818</v>
       </c>
       <c r="B18">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D18">
-        <v>40552</v>
+        <v>36847</v>
       </c>
       <c r="E18" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F18">
-        <v>106742</v>
+        <v>81736</v>
       </c>
       <c r="G18" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="H18">
         <v>223</v>
@@ -2162,24 +2157,24 @@
         <v>2</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L18">
-        <v>134608</v>
+        <v>74165</v>
       </c>
       <c r="M18" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19">
-        <v>571818</v>
+        <v>571819</v>
       </c>
       <c r="B19">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D19">
         <v>40552</v>
@@ -2188,22 +2183,25 @@
         <v>12</v>
       </c>
       <c r="F19">
-        <v>106742</v>
+        <v>133740</v>
       </c>
       <c r="G19" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H19">
-        <v>869</v>
+        <v>223</v>
       </c>
       <c r="I19" t="s">
-        <v>14</v>
+        <v>2</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="L19">
-        <v>106236</v>
+        <v>150091</v>
       </c>
       <c r="M19" t="s">
-        <v>137</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.45">
@@ -2217,244 +2215,247 @@
         <v>83</v>
       </c>
       <c r="D20">
-        <v>40552</v>
+        <v>107813</v>
       </c>
       <c r="E20" t="s">
-        <v>12</v>
+        <v>180</v>
       </c>
       <c r="F20">
-        <v>106742</v>
+        <v>36020</v>
       </c>
       <c r="G20" t="s">
-        <v>16</v>
+        <v>171</v>
       </c>
       <c r="H20">
-        <v>869</v>
+        <v>589</v>
       </c>
       <c r="I20" t="s">
-        <v>14</v>
+        <v>159</v>
       </c>
       <c r="L20">
-        <v>145535</v>
+        <v>164029</v>
       </c>
       <c r="M20" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21">
-        <v>571818</v>
+        <v>571816</v>
       </c>
       <c r="B21">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D21">
-        <v>40552</v>
+        <v>37669</v>
       </c>
       <c r="E21" t="s">
-        <v>12</v>
+        <v>275</v>
       </c>
       <c r="F21">
-        <v>106742</v>
+        <v>137918</v>
       </c>
       <c r="G21" t="s">
-        <v>16</v>
+        <v>161</v>
       </c>
       <c r="H21">
-        <v>869</v>
+        <v>1181</v>
       </c>
       <c r="I21" t="s">
-        <v>14</v>
+        <v>156</v>
       </c>
       <c r="L21">
-        <v>120827</v>
+        <v>22011</v>
       </c>
       <c r="M21" t="s">
-        <v>15</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22">
-        <v>571818</v>
+        <v>571817</v>
       </c>
       <c r="B22">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D22">
-        <v>53415</v>
+        <v>40202</v>
       </c>
       <c r="E22" t="s">
-        <v>179</v>
+        <v>76</v>
       </c>
       <c r="F22">
-        <v>146271</v>
+        <v>130214</v>
       </c>
       <c r="G22" t="s">
-        <v>168</v>
+        <v>71</v>
       </c>
       <c r="H22">
-        <v>1181</v>
+        <v>875</v>
       </c>
       <c r="I22" t="s">
-        <v>156</v>
+        <v>38</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>191</v>
+        <v>88</v>
       </c>
       <c r="L22">
-        <v>128776</v>
+        <v>51513</v>
       </c>
       <c r="M22" t="s">
-        <v>112</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23">
-        <v>571818</v>
+        <v>571819</v>
       </c>
       <c r="B23">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D23">
-        <v>53415</v>
+        <v>39883</v>
       </c>
       <c r="E23" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="F23">
-        <v>146271</v>
+        <v>44643</v>
       </c>
       <c r="G23" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H23">
-        <v>1181</v>
+        <v>1198</v>
       </c>
       <c r="I23" t="s">
-        <v>156</v>
+        <v>157</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>192</v>
       </c>
       <c r="L23">
-        <v>107006</v>
+        <v>129688</v>
       </c>
       <c r="M23" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24">
-        <v>571818</v>
+        <v>571819</v>
       </c>
       <c r="B24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D24">
-        <v>56148</v>
+        <v>18663</v>
       </c>
       <c r="E24" t="s">
-        <v>9</v>
+        <v>176</v>
       </c>
       <c r="F24">
-        <v>116676</v>
+        <v>126798</v>
       </c>
       <c r="G24" t="s">
-        <v>69</v>
+        <v>166</v>
       </c>
       <c r="H24">
-        <v>223</v>
+        <v>594</v>
       </c>
       <c r="I24" t="s">
-        <v>2</v>
+        <v>158</v>
       </c>
       <c r="L24">
-        <v>69830</v>
+        <v>151413</v>
       </c>
       <c r="M24" t="s">
-        <v>41</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25">
-        <v>571816</v>
+        <v>571819</v>
       </c>
       <c r="B25">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D25">
-        <v>56148</v>
+        <v>36847</v>
       </c>
       <c r="E25" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F25">
-        <v>116676</v>
+        <v>102597</v>
       </c>
       <c r="G25" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="H25">
-        <v>114</v>
+        <v>223</v>
       </c>
       <c r="I25" t="s">
-        <v>10</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>87</v>
+        <v>2</v>
       </c>
       <c r="L25">
-        <v>40406</v>
+        <v>169475</v>
       </c>
       <c r="M25" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26">
-        <v>571816</v>
+        <v>571818</v>
       </c>
       <c r="B26">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D26">
-        <v>37669</v>
+        <v>39883</v>
       </c>
       <c r="E26" t="s">
         <v>174</v>
       </c>
       <c r="F26">
-        <v>137918</v>
+        <v>139483</v>
       </c>
       <c r="G26" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H26">
-        <v>1181</v>
+        <v>1198</v>
       </c>
       <c r="I26" t="s">
-        <v>156</v>
+        <v>157</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>187</v>
       </c>
       <c r="L26">
-        <v>22011</v>
+        <v>134138</v>
       </c>
       <c r="M26" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.45">
@@ -2468,101 +2469,104 @@
         <v>83</v>
       </c>
       <c r="D27">
-        <v>18663</v>
+        <v>39883</v>
       </c>
       <c r="E27" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F27">
-        <v>126798</v>
+        <v>44643</v>
       </c>
       <c r="G27" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="H27">
-        <v>594</v>
+        <v>1198</v>
       </c>
       <c r="I27" t="s">
-        <v>158</v>
+        <v>157</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>192</v>
       </c>
       <c r="L27">
-        <v>151413</v>
+        <v>129079</v>
       </c>
       <c r="M27" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28">
-        <v>571818</v>
+        <v>571819</v>
       </c>
       <c r="B28">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D28">
-        <v>18663</v>
+        <v>39883</v>
       </c>
       <c r="E28" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F28">
-        <v>126798</v>
+        <v>44643</v>
       </c>
       <c r="G28" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="H28">
-        <v>594</v>
+        <v>628</v>
       </c>
       <c r="I28" t="s">
-        <v>158</v>
+        <v>66</v>
       </c>
       <c r="L28">
-        <v>164002</v>
+        <v>120917</v>
       </c>
       <c r="M28" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29">
-        <v>571817</v>
+        <v>571818</v>
       </c>
       <c r="B29">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D29">
-        <v>40202</v>
+        <v>40552</v>
       </c>
       <c r="E29" t="s">
-        <v>76</v>
+        <v>12</v>
       </c>
       <c r="F29">
-        <v>130214</v>
+        <v>133740</v>
       </c>
       <c r="G29" t="s">
-        <v>71</v>
+        <v>13</v>
       </c>
       <c r="H29">
-        <v>875</v>
+        <v>869</v>
       </c>
       <c r="I29" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>88</v>
+        <v>189</v>
       </c>
       <c r="L29">
-        <v>51513</v>
+        <v>162160</v>
       </c>
       <c r="M29" t="s">
-        <v>37</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.45">
@@ -2576,31 +2580,31 @@
         <v>82</v>
       </c>
       <c r="D30">
-        <v>36847</v>
+        <v>40552</v>
       </c>
       <c r="E30" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F30">
-        <v>81736</v>
+        <v>133740</v>
       </c>
       <c r="G30" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="H30">
-        <v>223</v>
+        <v>1198</v>
       </c>
       <c r="I30" t="s">
-        <v>2</v>
+        <v>157</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>92</v>
+        <v>188</v>
       </c>
       <c r="L30">
-        <v>74165</v>
+        <v>107961</v>
       </c>
       <c r="M30" t="s">
-        <v>19</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.45">
@@ -2614,16 +2618,16 @@
         <v>82</v>
       </c>
       <c r="D31">
-        <v>36847</v>
+        <v>40552</v>
       </c>
       <c r="E31" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F31">
-        <v>81736</v>
+        <v>133740</v>
       </c>
       <c r="G31" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="H31">
         <v>223</v>
@@ -2632,33 +2636,33 @@
         <v>2</v>
       </c>
       <c r="L31">
-        <v>129881</v>
+        <v>150025</v>
       </c>
       <c r="M31" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A32">
-        <v>571816</v>
+        <v>571819</v>
       </c>
       <c r="B32">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D32">
-        <v>36847</v>
+        <v>40552</v>
       </c>
       <c r="E32" t="s">
-        <v>0</v>
-      </c>
-      <c r="F32">
-        <v>81736</v>
-      </c>
-      <c r="G32" t="s">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="F32" s="6">
+        <v>99</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>274</v>
       </c>
       <c r="H32">
         <v>223</v>
@@ -2666,151 +2670,157 @@
       <c r="I32" t="s">
         <v>2</v>
       </c>
+      <c r="J32" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="L32">
-        <v>38739</v>
+        <v>134608</v>
       </c>
       <c r="M32" t="s">
-        <v>133</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A33">
-        <v>571819</v>
+        <v>571818</v>
       </c>
       <c r="B33">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D33">
-        <v>36847</v>
+        <v>40552</v>
       </c>
       <c r="E33" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F33">
-        <v>93110</v>
+        <v>106742</v>
       </c>
       <c r="G33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H33">
-        <v>223</v>
+        <v>869</v>
       </c>
       <c r="I33" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="L33">
-        <v>145200</v>
+        <v>106236</v>
       </c>
       <c r="M33" t="s">
-        <v>106</v>
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A34">
-        <v>571819</v>
+        <v>571818</v>
       </c>
       <c r="B34">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D34">
-        <v>36847</v>
+        <v>53415</v>
       </c>
       <c r="E34" t="s">
-        <v>0</v>
+        <v>178</v>
       </c>
       <c r="F34">
-        <v>93110</v>
+        <v>146271</v>
       </c>
       <c r="G34" t="s">
-        <v>17</v>
+        <v>168</v>
       </c>
       <c r="H34">
-        <v>223</v>
+        <v>1181</v>
       </c>
       <c r="I34" t="s">
-        <v>2</v>
+        <v>156</v>
       </c>
       <c r="L34">
-        <v>101580</v>
+        <v>107006</v>
       </c>
       <c r="M34" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A35">
-        <v>571819</v>
+        <v>571816</v>
       </c>
       <c r="B35">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D35">
-        <v>36847</v>
+        <v>56148</v>
       </c>
       <c r="E35" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F35">
-        <v>93110</v>
+        <v>116676</v>
       </c>
       <c r="G35" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="H35">
-        <v>223</v>
+        <v>114</v>
       </c>
       <c r="I35" t="s">
-        <v>2</v>
+        <v>10</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="L35">
-        <v>145224</v>
+        <v>40406</v>
       </c>
       <c r="M35" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A36">
-        <v>571819</v>
+        <v>571818</v>
       </c>
       <c r="B36">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D36">
-        <v>36847</v>
+        <v>18663</v>
       </c>
       <c r="E36" t="s">
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="F36">
-        <v>102597</v>
+        <v>126798</v>
       </c>
       <c r="G36" t="s">
-        <v>42</v>
+        <v>166</v>
       </c>
       <c r="H36">
-        <v>223</v>
+        <v>594</v>
       </c>
       <c r="I36" t="s">
-        <v>2</v>
+        <v>158</v>
       </c>
       <c r="L36">
-        <v>169475</v>
+        <v>164002</v>
       </c>
       <c r="M36" t="s">
-        <v>26</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.45">
@@ -2830,10 +2840,10 @@
         <v>0</v>
       </c>
       <c r="F37">
-        <v>102597</v>
+        <v>81736</v>
       </c>
       <c r="G37" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="H37">
         <v>223</v>
@@ -2842,21 +2852,21 @@
         <v>2</v>
       </c>
       <c r="L37">
-        <v>109403</v>
+        <v>129881</v>
       </c>
       <c r="M37" t="s">
-        <v>20</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A38">
-        <v>571819</v>
+        <v>571816</v>
       </c>
       <c r="B38">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D38">
         <v>36847</v>
@@ -2865,10 +2875,10 @@
         <v>0</v>
       </c>
       <c r="F38">
-        <v>102597</v>
+        <v>81736</v>
       </c>
       <c r="G38" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="H38">
         <v>223</v>
@@ -2877,13 +2887,13 @@
         <v>2</v>
       </c>
       <c r="L38">
-        <v>155140</v>
+        <v>38739</v>
       </c>
       <c r="M38" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>571819</v>
       </c>
@@ -2894,107 +2904,98 @@
         <v>83</v>
       </c>
       <c r="D39">
-        <v>69289</v>
+        <v>36847</v>
       </c>
       <c r="E39" t="s">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="F39">
-        <v>126785</v>
+        <v>93110</v>
       </c>
       <c r="G39" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="H39">
-        <v>609</v>
+        <v>223</v>
       </c>
       <c r="I39" t="s">
-        <v>63</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>95</v>
+        <v>2</v>
       </c>
       <c r="L39">
-        <v>131893</v>
+        <v>101580</v>
       </c>
       <c r="M39" t="s">
-        <v>55</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A40">
-        <v>571816</v>
+        <v>571819</v>
       </c>
       <c r="B40">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C40" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D40">
-        <v>69289</v>
+        <v>36847</v>
       </c>
       <c r="E40" t="s">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="F40">
-        <v>126785</v>
+        <v>93110</v>
       </c>
       <c r="G40" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="H40">
-        <v>609</v>
+        <v>223</v>
       </c>
       <c r="I40" t="s">
-        <v>63</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>86</v>
+        <v>2</v>
       </c>
       <c r="L40">
-        <v>35251</v>
+        <v>145224</v>
       </c>
       <c r="M40" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A41">
-        <v>571819</v>
+        <v>571818</v>
       </c>
       <c r="B41">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D41">
-        <v>107813</v>
+        <v>36847</v>
       </c>
       <c r="E41" t="s">
-        <v>181</v>
+        <v>0</v>
       </c>
       <c r="F41">
-        <v>36020</v>
+        <v>102597</v>
       </c>
       <c r="G41" t="s">
-        <v>171</v>
+        <v>42</v>
       </c>
       <c r="H41">
-        <v>589</v>
+        <v>223</v>
       </c>
       <c r="I41" t="s">
-        <v>159</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>194</v>
+        <v>2</v>
       </c>
       <c r="L41">
-        <v>116705</v>
+        <v>109403</v>
       </c>
       <c r="M41" t="s">
-        <v>139</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.45">
@@ -3008,102 +3009,104 @@
         <v>83</v>
       </c>
       <c r="D42">
+        <v>36847</v>
+      </c>
+      <c r="E42" t="s">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>102597</v>
+      </c>
+      <c r="G42" t="s">
+        <v>42</v>
+      </c>
+      <c r="H42">
+        <v>223</v>
+      </c>
+      <c r="I42" t="s">
+        <v>2</v>
+      </c>
+      <c r="L42">
+        <v>155140</v>
+      </c>
+      <c r="M42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>571816</v>
+      </c>
+      <c r="B43">
+        <v>3</v>
+      </c>
+      <c r="C43" t="s">
+        <v>80</v>
+      </c>
+      <c r="D43">
+        <v>69289</v>
+      </c>
+      <c r="E43" t="s">
+        <v>74</v>
+      </c>
+      <c r="F43">
+        <v>126785</v>
+      </c>
+      <c r="G43" t="s">
+        <v>68</v>
+      </c>
+      <c r="H43">
+        <v>609</v>
+      </c>
+      <c r="I43" t="s">
+        <v>63</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="L43">
+        <v>35251</v>
+      </c>
+      <c r="M43" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>571819</v>
+      </c>
+      <c r="B44">
+        <v>6</v>
+      </c>
+      <c r="C44" t="s">
+        <v>83</v>
+      </c>
+      <c r="D44">
         <v>107813</v>
       </c>
-      <c r="E42" t="s">
-        <v>181</v>
-      </c>
-      <c r="F42">
+      <c r="E44" t="s">
+        <v>180</v>
+      </c>
+      <c r="F44">
         <v>36020</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G44" t="s">
         <v>171</v>
       </c>
-      <c r="H42">
+      <c r="H44">
         <v>589</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I44" t="s">
         <v>159</v>
       </c>
-      <c r="L42">
-        <v>164029</v>
-      </c>
-      <c r="M42" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="1">
-        <v>571818</v>
-      </c>
-      <c r="B43" s="1">
-        <v>5</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D43" s="1">
-        <v>27704</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="F43" s="1">
-        <v>62424</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="H43" s="1">
-        <v>589</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="J43" s="3"/>
-      <c r="L43" s="1">
-        <v>141796</v>
-      </c>
-      <c r="M43" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A44">
-        <v>571817</v>
-      </c>
-      <c r="B44">
-        <v>4</v>
-      </c>
-      <c r="C44" t="s">
-        <v>81</v>
-      </c>
-      <c r="D44">
-        <v>54412</v>
-      </c>
-      <c r="E44" t="s">
-        <v>75</v>
-      </c>
-      <c r="F44">
-        <v>51273</v>
-      </c>
-      <c r="G44" t="s">
-        <v>70</v>
-      </c>
-      <c r="H44">
-        <v>579</v>
-      </c>
-      <c r="I44" t="s">
-        <v>64</v>
-      </c>
       <c r="J44" s="2" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="L44">
-        <v>128692</v>
+        <v>116705</v>
       </c>
       <c r="M44" t="s">
-        <v>53</v>
+        <v>139</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.45">
@@ -3266,7 +3269,7 @@
         <v>18663</v>
       </c>
       <c r="E49" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F49">
         <v>126798</v>
@@ -3319,7 +3322,7 @@
         <v>96</v>
       </c>
       <c r="K50" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L50">
         <v>179705</v>
@@ -3372,7 +3375,7 @@
         <v>59650</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F51" s="6">
         <v>81536</v>
@@ -3407,7 +3410,7 @@
         <v>18663</v>
       </c>
       <c r="E52" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F52">
         <v>126798</v>
@@ -3442,7 +3445,7 @@
         <v>103897</v>
       </c>
       <c r="E53" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F53">
         <v>166762</v>
@@ -3457,10 +3460,10 @@
         <v>158</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K53" s="6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="L53">
         <v>177919</v>
@@ -3507,7 +3510,7 @@
         <v>103897</v>
       </c>
       <c r="E54" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F54">
         <v>166762</v>
@@ -3522,10 +3525,10 @@
         <v>158</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K54" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="L54">
         <v>170947</v>
@@ -3581,7 +3584,7 @@
         <v>65</v>
       </c>
       <c r="K55" s="6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="L55">
         <v>176931</v>
@@ -3605,7 +3608,7 @@
         <v>11</v>
       </c>
       <c r="S55" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.45">
@@ -3622,7 +3625,7 @@
         <v>27704</v>
       </c>
       <c r="E56" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F56">
         <v>62424</v>
@@ -3637,7 +3640,7 @@
         <v>159</v>
       </c>
       <c r="K56" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="L56">
         <v>166499</v>
@@ -3684,7 +3687,7 @@
         <v>102</v>
       </c>
       <c r="K57" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="L57">
         <v>112424</v>
@@ -3710,16 +3713,16 @@
         <v>101</v>
       </c>
       <c r="D58" s="6">
-        <v>53415</v>
+        <v>37669</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>179</v>
+        <v>275</v>
       </c>
       <c r="F58" s="6">
         <v>109835</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H58" s="6">
         <v>1181</v>
@@ -3728,19 +3731,19 @@
         <v>156</v>
       </c>
       <c r="K58" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L58" s="6">
         <v>68011</v>
       </c>
       <c r="M58" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="N58" s="6">
         <v>40518</v>
       </c>
       <c r="O58" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.45">
@@ -3809,13 +3812,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D1">
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
@@ -3826,13 +3829,13 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D2">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -3843,13 +3846,13 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D3">
         <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -3860,13 +3863,13 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D4">
         <v>1063</v>
       </c>
       <c r="F4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -3877,13 +3880,13 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D5">
         <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
@@ -3894,13 +3897,13 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D6">
         <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
@@ -3911,13 +3914,13 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D7">
         <v>30</v>
       </c>
       <c r="F7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
@@ -3934,7 +3937,7 @@
         <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
@@ -3951,7 +3954,7 @@
         <v>1061</v>
       </c>
       <c r="F9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
@@ -3968,7 +3971,7 @@
         <v>34</v>
       </c>
       <c r="F10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
@@ -3985,7 +3988,7 @@
         <v>38</v>
       </c>
       <c r="F11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
@@ -4002,10 +4005,10 @@
         <v>42</v>
       </c>
       <c r="E12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
@@ -4022,7 +4025,7 @@
         <v>43</v>
       </c>
       <c r="E13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
@@ -4039,10 +4042,10 @@
         <v>1053</v>
       </c>
       <c r="E14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
@@ -4059,10 +4062,10 @@
         <v>47</v>
       </c>
       <c r="E15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
@@ -4079,10 +4082,10 @@
         <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
@@ -4099,7 +4102,7 @@
         <v>1058</v>
       </c>
       <c r="E17" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
@@ -4110,13 +4113,13 @@
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D18">
         <v>1065</v>
       </c>
       <c r="F18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -4129,7 +4132,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4167,7 +4170,7 @@
         <v>37669</v>
       </c>
       <c r="B4" t="s">
-        <v>174</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
@@ -4175,7 +4178,7 @@
         <v>39883</v>
       </c>
       <c r="B5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
@@ -4183,7 +4186,7 @@
         <v>40068</v>
       </c>
       <c r="B6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
@@ -4191,7 +4194,7 @@
         <v>18663</v>
       </c>
       <c r="B7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
@@ -4247,7 +4250,7 @@
         <v>27704</v>
       </c>
       <c r="B14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
@@ -4255,7 +4258,7 @@
         <v>53415</v>
       </c>
       <c r="B15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
@@ -4263,7 +4266,7 @@
         <v>59650</v>
       </c>
       <c r="B16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
@@ -4271,7 +4274,7 @@
         <v>107813</v>
       </c>
       <c r="B17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
@@ -4287,7 +4290,7 @@
         <v>103897</v>
       </c>
       <c r="B19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -4297,10 +4300,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E50BA4F-C9F6-4C5B-8947-232726082284}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:B21"/>
+      <selection activeCell="A28" sqref="A28:B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4522,7 +4525,15 @@
         <v>109835</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A28" s="6">
+        <v>99</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -4711,7 +4722,7 @@
         <v>141</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -4719,7 +4730,7 @@
         <v>68011</v>
       </c>
       <c r="B3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
@@ -4738,7 +4749,7 @@
         <v>140</v>
       </c>
       <c r="C5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
@@ -4749,7 +4760,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
@@ -4760,7 +4771,7 @@
         <v>136</v>
       </c>
       <c r="C7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
@@ -4771,7 +4782,7 @@
         <v>53</v>
       </c>
       <c r="C8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
@@ -4806,7 +4817,7 @@
         <v>142</v>
       </c>
       <c r="C12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
@@ -4849,7 +4860,7 @@
         <v>138</v>
       </c>
       <c r="C17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
@@ -4860,7 +4871,7 @@
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
@@ -4871,7 +4882,7 @@
         <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
@@ -4882,7 +4893,7 @@
         <v>119</v>
       </c>
       <c r="C20" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
@@ -4893,7 +4904,7 @@
         <v>108</v>
       </c>
       <c r="C21" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
@@ -4928,7 +4939,7 @@
         <v>55</v>
       </c>
       <c r="C25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
@@ -4936,7 +4947,7 @@
         <v>40518</v>
       </c>
       <c r="B26" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
@@ -4947,7 +4958,7 @@
         <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
@@ -4974,7 +4985,7 @@
         <v>37</v>
       </c>
       <c r="C30" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
@@ -5033,7 +5044,7 @@
         <v>23</v>
       </c>
       <c r="C37" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.45">
@@ -5060,7 +5071,7 @@
         <v>52</v>
       </c>
       <c r="C40" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.45">
@@ -5079,7 +5090,7 @@
         <v>50</v>
       </c>
       <c r="C42" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.45">
@@ -5090,7 +5101,7 @@
         <v>129</v>
       </c>
       <c r="C43" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.45">
@@ -5101,7 +5112,7 @@
         <v>133</v>
       </c>
       <c r="C44" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.45">
@@ -5120,7 +5131,7 @@
         <v>113</v>
       </c>
       <c r="C46" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.45">
@@ -5139,7 +5150,7 @@
         <v>6</v>
       </c>
       <c r="C48" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.45">
@@ -5166,7 +5177,7 @@
         <v>97</v>
       </c>
       <c r="C51" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="52" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.45">
@@ -5177,7 +5188,7 @@
         <v>126</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="53" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.45">
@@ -5188,7 +5199,7 @@
         <v>4</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="54" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.45">
@@ -5223,7 +5234,7 @@
         <v>106</v>
       </c>
       <c r="C57" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.45">
@@ -5250,7 +5261,7 @@
         <v>128</v>
       </c>
       <c r="C60" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.45">
@@ -5269,7 +5280,7 @@
         <v>15</v>
       </c>
       <c r="C62" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.45">
@@ -5336,7 +5347,7 @@
         <v>26</v>
       </c>
       <c r="C70" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.45">
@@ -5344,7 +5355,7 @@
         <v>11</v>
       </c>
       <c r="B71" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.45">
@@ -5355,7 +5366,7 @@
         <v>137</v>
       </c>
       <c r="C72" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.45">
@@ -5374,7 +5385,7 @@
         <v>21</v>
       </c>
       <c r="C74" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.45">
@@ -5385,7 +5396,7 @@
         <v>118</v>
       </c>
       <c r="C75" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.45">
@@ -5396,7 +5407,7 @@
         <v>41</v>
       </c>
       <c r="C76" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.45">
@@ -5407,7 +5418,7 @@
         <v>112</v>
       </c>
       <c r="C77" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.45">
@@ -5418,7 +5429,7 @@
         <v>117</v>
       </c>
       <c r="C78" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.45">
@@ -5437,7 +5448,7 @@
         <v>139</v>
       </c>
       <c r="C80" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.45">
@@ -5456,7 +5467,7 @@
         <v>116</v>
       </c>
       <c r="C82" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.45">
@@ -5483,7 +5494,7 @@
         <v>134</v>
       </c>
       <c r="C85" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.45">
@@ -5494,7 +5505,7 @@
         <v>127</v>
       </c>
       <c r="C86" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.45">
@@ -5505,7 +5516,7 @@
         <v>20</v>
       </c>
       <c r="C87" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.45">
@@ -5516,7 +5527,7 @@
         <v>115</v>
       </c>
       <c r="C88" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.45">
@@ -5527,7 +5538,7 @@
         <v>62</v>
       </c>
       <c r="C89" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.45">
@@ -5538,7 +5549,7 @@
         <v>135</v>
       </c>
       <c r="C90" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.45">
@@ -5557,7 +5568,7 @@
         <v>54</v>
       </c>
       <c r="C92" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.45">
@@ -5568,7 +5579,7 @@
         <v>18</v>
       </c>
       <c r="C93" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.45">
@@ -5587,7 +5598,7 @@
         <v>19</v>
       </c>
       <c r="C95" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.45">

</xml_diff>